<commit_message>
Hikvision file has been updated
</commit_message>
<xml_diff>
--- a/HIKVISION JUNE 2021 PRICE LIST (MOP).xlsx
+++ b/HIKVISION JUNE 2021 PRICE LIST (MOP).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\easo mathew\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meljo scans\AWS related\DEvOps 1\DEVOPSGITTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="HD DVR" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="EZVIZ" sheetId="7" r:id="rId7"/>
     <sheet name="BIOMETRIC" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="441">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1430,6 +1431,9 @@
   </si>
   <si>
     <t>CAMERA</t>
+  </si>
+  <si>
+    <t>Hello this is a test file updation. Git is here.</t>
   </si>
 </sst>
 </file>
@@ -2876,6 +2880,7 @@
     <xf numFmtId="0" fontId="92" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2924,6 +2929,30 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2942,39 +2971,33 @@
     <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3023,24 +3046,6 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3095,7 +3100,6 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3135,7 +3139,7 @@
         <xdr:cNvPr id="2757" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F794545B-F0AD-4D5E-A9B7-5F7DD3D743EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F794545B-F0AD-4D5E-A9B7-5F7DD3D743EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3209,7 +3213,7 @@
         <xdr:cNvPr id="2758" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D3C60F-939C-4EB5-9518-224E25F16960}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15D3C60F-939C-4EB5-9518-224E25F16960}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3288,7 +3292,7 @@
         <xdr:cNvPr id="14564" name="Picture 10" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F450D326-A10A-4C17-932A-29E325E7772B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F450D326-A10A-4C17-932A-29E325E7772B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3362,7 +3366,7 @@
         <xdr:cNvPr id="14565" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B7163B-A39D-4579-BF37-31F72DF3A3E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B7163B-A39D-4579-BF37-31F72DF3A3E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3436,7 +3440,7 @@
         <xdr:cNvPr id="14566" name="Picture 12" descr="Image result for CS-X5C-4APEC">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEF73321-D25C-4263-A062-A8A4A50B64A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEF73321-D25C-4263-A062-A8A4A50B64A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3510,7 +3514,7 @@
         <xdr:cNvPr id="14567" name="Picture 13" descr="Image result for C1C CAMERA">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FABD93E-A38C-433B-ACE6-ABABF15DE2DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4FABD93E-A38C-433B-ACE6-ABABF15DE2DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3584,7 +3588,7 @@
         <xdr:cNvPr id="14568" name="Picture 14" descr="Image result for CS-CV346-AO-7A3WFR(3MP)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77CFCDF6-B04D-4EC4-AC5D-ED82A54AB919}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{77CFCDF6-B04D-4EC4-AC5D-ED82A54AB919}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3658,7 +3662,7 @@
         <xdr:cNvPr id="14569" name="Picture 15" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F14B0F-DD82-40C8-B42B-F711EB4B66F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A2F14B0F-DD82-40C8-B42B-F711EB4B66F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3732,7 +3736,7 @@
         <xdr:cNvPr id="14570" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45B85A1-918B-48CB-9D61-7AB33CABEF38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A45B85A1-918B-48CB-9D61-7AB33CABEF38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3806,7 +3810,7 @@
         <xdr:cNvPr id="14571" name="Picture 15" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6B0AD6D-C36D-4E0A-81DD-DF43FC954379}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6B0AD6D-C36D-4E0A-81DD-DF43FC954379}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3880,7 +3884,7 @@
         <xdr:cNvPr id="14572" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2C1C4E-39B8-419D-8C58-48DCE0C63BA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB2C1C4E-39B8-419D-8C58-48DCE0C63BA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3954,7 +3958,7 @@
         <xdr:cNvPr id="14573" name="AutoShape 3" descr="Image result for CS-CV310-A0-1B2WFR">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58FE2307-73C2-4B94-A8A4-6F0CE4F0ACFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{58FE2307-73C2-4B94-A8A4-6F0CE4F0ACFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4015,7 +4019,7 @@
         <xdr:cNvPr id="14574" name="Picture 13" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7080737-A6C9-4FBB-B8A4-29BA5D8D30DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B7080737-A6C9-4FBB-B8A4-29BA5D8D30DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4089,7 +4093,7 @@
         <xdr:cNvPr id="14575" name="Picture 15" descr="Image result for C1C CAMERA">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0B5B8F1-63F4-4958-B1D3-30B9BA7F7815}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E0B5B8F1-63F4-4958-B1D3-30B9BA7F7815}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4163,7 +4167,7 @@
         <xdr:cNvPr id="14576" name="Picture 16" descr="Image result for CS-CV346-AO-7A3WFR(3MP)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2ED700-160A-4191-A9B9-F382F2F9E451}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CF2ED700-160A-4191-A9B9-F382F2F9E451}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4237,7 +4241,7 @@
         <xdr:cNvPr id="14577" name="Picture 17" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBFB5773-8A75-4665-AC47-44CC01BB972B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBFB5773-8A75-4665-AC47-44CC01BB972B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4311,7 +4315,7 @@
         <xdr:cNvPr id="14578" name="Picture 18" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E035C21-C91C-4651-B4FD-A1ECA30E860D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E035C21-C91C-4651-B4FD-A1ECA30E860D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4385,7 +4389,7 @@
         <xdr:cNvPr id="14579" name="Picture 19" descr="Image result for EZVIZ NVR KIT">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397FF8EE-BFB2-4FE7-A3B2-F9942321552C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{397FF8EE-BFB2-4FE7-A3B2-F9942321552C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4459,7 +4463,7 @@
         <xdr:cNvPr id="14580" name="Picture 20" descr="Camera IP EZVIZ CS-C3N (A0-3H2WFRL) 1080P Có Màu Ban Đêm - Hàng ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B46A902-DED4-4EA9-A473-659B44C1B7AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B46A902-DED4-4EA9-A473-659B44C1B7AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4533,7 +4537,7 @@
         <xdr:cNvPr id="14581" name="Picture 21" descr="Camera IP EZVIZ CS-C3N (A0-3H2WFRL) 1080P Có Màu Ban Đêm - Hàng ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691C9B81-B5BB-4F80-A630-EAF4F98C6EB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{691C9B81-B5BB-4F80-A630-EAF4F98C6EB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4607,7 +4611,7 @@
         <xdr:cNvPr id="14582" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7354854F-34EB-4903-A01B-7844B435C044}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7354854F-34EB-4903-A01B-7844B435C044}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4973,22 +4977,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="2:17" ht="86.25" customHeight="1">
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="32" t="s">
@@ -5000,10 +5004,10 @@
       <c r="F3" s="41"/>
     </row>
     <row r="4" spans="2:17" ht="23.25">
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="180" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="180"/>
+      <c r="C4" s="181"/>
     </row>
     <row r="5" spans="2:17" ht="15.75">
       <c r="B5" s="128" t="s">
@@ -5012,7 +5016,7 @@
       <c r="C5" s="84">
         <v>2900</v>
       </c>
-      <c r="G5" s="177"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="2:17" ht="15.75">
       <c r="B6" s="128" t="s">
@@ -5021,11 +5025,11 @@
       <c r="C6" s="84">
         <v>4340</v>
       </c>
-      <c r="G6" s="177"/>
-      <c r="P6" s="169" t="s">
+      <c r="G6" s="178"/>
+      <c r="P6" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="Q6" s="169"/>
+      <c r="Q6" s="170"/>
     </row>
     <row r="7" spans="2:17" ht="15.75">
       <c r="B7" s="128" t="s">
@@ -5034,7 +5038,7 @@
       <c r="C7" s="84">
         <v>7550</v>
       </c>
-      <c r="G7" s="177"/>
+      <c r="G7" s="178"/>
       <c r="O7" s="11" t="s">
         <v>39</v>
       </c>
@@ -5046,10 +5050,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" ht="23.25">
-      <c r="B8" s="181" t="s">
+      <c r="B8" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="182"/>
+      <c r="C8" s="183"/>
       <c r="G8" s="25"/>
       <c r="O8" s="11"/>
       <c r="P8" s="42"/>
@@ -5062,7 +5066,7 @@
       <c r="C9" s="130">
         <v>2350</v>
       </c>
-      <c r="G9" s="178" t="s">
+      <c r="G9" s="179" t="s">
         <v>66</v>
       </c>
       <c r="O9" s="11"/>
@@ -5076,7 +5080,7 @@
       <c r="C10" s="130">
         <v>3550</v>
       </c>
-      <c r="G10" s="178"/>
+      <c r="G10" s="179"/>
       <c r="O10" s="11"/>
       <c r="P10" s="42"/>
       <c r="Q10" s="11"/>
@@ -5088,7 +5092,7 @@
       <c r="C11" s="130">
         <v>5950</v>
       </c>
-      <c r="G11" s="178"/>
+      <c r="G11" s="179"/>
       <c r="O11" s="11"/>
       <c r="P11" s="42"/>
       <c r="Q11" s="11"/>
@@ -5100,7 +5104,7 @@
       <c r="C12" s="130">
         <v>5950</v>
       </c>
-      <c r="G12" s="178"/>
+      <c r="G12" s="179"/>
       <c r="O12" s="11"/>
       <c r="P12" s="42"/>
       <c r="Q12" s="11"/>
@@ -5112,7 +5116,7 @@
       <c r="C13" s="130">
         <v>8200</v>
       </c>
-      <c r="G13" s="178"/>
+      <c r="G13" s="179"/>
       <c r="O13" s="11"/>
       <c r="P13" s="42"/>
       <c r="Q13" s="11"/>
@@ -5124,17 +5128,17 @@
       <c r="C14" s="130">
         <v>17500</v>
       </c>
-      <c r="G14" s="178"/>
+      <c r="G14" s="179"/>
       <c r="O14" s="43"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="43"/>
     </row>
     <row r="15" spans="2:17" ht="23.25">
-      <c r="B15" s="181" t="s">
+      <c r="B15" s="182" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="182"/>
-      <c r="G15" s="178"/>
+      <c r="C15" s="183"/>
+      <c r="G15" s="179"/>
       <c r="P15" s="41"/>
     </row>
     <row r="16" spans="2:17" ht="15.75">
@@ -5144,7 +5148,7 @@
       <c r="C16" s="130">
         <v>10500</v>
       </c>
-      <c r="G16" s="178"/>
+      <c r="G16" s="179"/>
       <c r="P16" s="41"/>
     </row>
     <row r="17" spans="2:16" ht="15.75">
@@ -5154,7 +5158,7 @@
       <c r="C17" s="130">
         <v>14500</v>
       </c>
-      <c r="G17" s="178"/>
+      <c r="G17" s="179"/>
       <c r="P17" s="41"/>
     </row>
     <row r="18" spans="2:16" ht="15.75">
@@ -5164,7 +5168,7 @@
       <c r="C18" s="130">
         <v>3900</v>
       </c>
-      <c r="G18" s="178"/>
+      <c r="G18" s="179"/>
       <c r="P18" s="41"/>
     </row>
     <row r="19" spans="2:16" ht="15.75">
@@ -5174,7 +5178,7 @@
       <c r="C19" s="130">
         <v>5720</v>
       </c>
-      <c r="G19" s="178"/>
+      <c r="G19" s="179"/>
       <c r="P19" s="41"/>
     </row>
     <row r="20" spans="2:16" ht="15.75">
@@ -5184,7 +5188,7 @@
       <c r="C20" s="130">
         <v>9800</v>
       </c>
-      <c r="G20" s="178"/>
+      <c r="G20" s="179"/>
       <c r="P20" s="41"/>
     </row>
     <row r="21" spans="2:16" ht="15.75">
@@ -5194,7 +5198,7 @@
       <c r="C21" s="130">
         <v>7900</v>
       </c>
-      <c r="G21" s="178"/>
+      <c r="G21" s="179"/>
       <c r="P21" s="41"/>
     </row>
     <row r="22" spans="2:16" ht="15.75">
@@ -5204,15 +5208,15 @@
       <c r="C22" s="130">
         <v>11500</v>
       </c>
-      <c r="G22" s="178"/>
+      <c r="G22" s="179"/>
       <c r="P22" s="41"/>
     </row>
     <row r="23" spans="2:16" ht="20.25">
-      <c r="B23" s="183" t="s">
+      <c r="B23" s="184" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="184"/>
-      <c r="G23" s="178"/>
+      <c r="C23" s="185"/>
+      <c r="G23" s="179"/>
       <c r="P23" s="41"/>
     </row>
     <row r="24" spans="2:16" ht="15.75">
@@ -5222,7 +5226,7 @@
       <c r="C24" s="84" t="s">
         <v>384</v>
       </c>
-      <c r="G24" s="178"/>
+      <c r="G24" s="179"/>
       <c r="P24" s="41"/>
     </row>
     <row r="25" spans="2:16" ht="15.75">
@@ -5232,7 +5236,7 @@
       <c r="C25" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="G25" s="178"/>
+      <c r="G25" s="179"/>
       <c r="P25" s="41"/>
     </row>
     <row r="26" spans="2:16" ht="15.75">
@@ -5242,7 +5246,7 @@
       <c r="C26" s="84">
         <v>0</v>
       </c>
-      <c r="G26" s="178"/>
+      <c r="G26" s="179"/>
       <c r="P26" s="41"/>
     </row>
     <row r="27" spans="2:16" ht="15.75">
@@ -5252,7 +5256,7 @@
       <c r="C27" s="84" t="s">
         <v>386</v>
       </c>
-      <c r="G27" s="178"/>
+      <c r="G27" s="179"/>
       <c r="P27" s="41"/>
     </row>
     <row r="28" spans="2:16" ht="15.75">
@@ -5262,7 +5266,7 @@
       <c r="C28" s="84">
         <v>17000</v>
       </c>
-      <c r="G28" s="178"/>
+      <c r="G28" s="179"/>
     </row>
     <row r="29" spans="2:16" ht="15.75">
       <c r="B29" s="128" t="s">
@@ -5274,10 +5278,10 @@
       <c r="G29" s="40"/>
     </row>
     <row r="30" spans="2:16" ht="26.25">
-      <c r="B30" s="172" t="s">
+      <c r="B30" s="173" t="s">
         <v>276</v>
       </c>
-      <c r="C30" s="173"/>
+      <c r="C30" s="174"/>
     </row>
     <row r="31" spans="2:16" ht="15.75">
       <c r="B31" s="131" t="s">
@@ -5296,10 +5300,10 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="20.25">
-      <c r="B35" s="176" t="s">
+      <c r="B35" s="177" t="s">
         <v>152</v>
       </c>
-      <c r="C35" s="176"/>
+      <c r="C35" s="177"/>
     </row>
     <row r="36" spans="2:4" ht="15.75">
       <c r="B36" s="86" t="s">
@@ -5330,10 +5334,10 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="20.25">
-      <c r="B40" s="170" t="s">
+      <c r="B40" s="171" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="170"/>
+      <c r="C40" s="171"/>
     </row>
     <row r="41" spans="2:4" ht="15.75">
       <c r="B41" s="131" t="s">
@@ -5358,10 +5362,10 @@
       <c r="C43" s="132"/>
     </row>
     <row r="45" spans="2:4" ht="18">
-      <c r="B45" s="171" t="s">
+      <c r="B45" s="172" t="s">
         <v>154</v>
       </c>
-      <c r="C45" s="171"/>
+      <c r="C45" s="172"/>
     </row>
     <row r="46" spans="2:4" ht="15.75">
       <c r="B46" s="131" t="s">
@@ -5412,6 +5416,24 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5437,39 +5459,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="2:10" ht="87.75" customHeight="1">
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="2:10" ht="15.75">
       <c r="B3" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="35"/>
-      <c r="H3" s="191" t="s">
+      <c r="H3" s="186" t="s">
         <v>431</v>
       </c>
-      <c r="I3" s="191"/>
-      <c r="J3" s="191"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="186"/>
     </row>
     <row r="4" spans="2:10" ht="26.25">
-      <c r="B4" s="194" t="s">
+      <c r="B4" s="189" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="195"/>
+      <c r="C4" s="190"/>
       <c r="H4" s="45" t="s">
         <v>337</v>
       </c>
@@ -5537,11 +5559,11 @@
       <c r="C9" s="130">
         <v>1600</v>
       </c>
-      <c r="H9" s="192" t="s">
+      <c r="H9" s="187" t="s">
         <v>341</v>
       </c>
-      <c r="I9" s="192"/>
-      <c r="J9" s="192"/>
+      <c r="I9" s="187"/>
+      <c r="J9" s="187"/>
     </row>
     <row r="10" spans="2:10" ht="30">
       <c r="B10" s="141" t="s">
@@ -5619,10 +5641,10 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="27">
-      <c r="B16" s="196" t="s">
+      <c r="B16" s="191" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="197"/>
+      <c r="C16" s="192"/>
     </row>
     <row r="17" spans="2:3" ht="17.25">
       <c r="B17" s="142" t="s">
@@ -5773,10 +5795,10 @@
       <c r="C35" s="12"/>
     </row>
     <row r="36" spans="2:3" ht="20.25">
-      <c r="B36" s="198" t="s">
+      <c r="B36" s="193" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="198"/>
+      <c r="C36" s="193"/>
     </row>
     <row r="37" spans="2:3" ht="15.75">
       <c r="B37" s="146" t="s">
@@ -5875,10 +5897,10 @@
       <c r="C49" s="1"/>
     </row>
     <row r="51" spans="2:16" ht="23.25">
-      <c r="B51" s="193" t="s">
+      <c r="B51" s="188" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="193"/>
+      <c r="C51" s="188"/>
     </row>
     <row r="52" spans="2:16" ht="17.25">
       <c r="B52" s="141" t="s">
@@ -5927,10 +5949,10 @@
       <c r="C57" s="140">
         <v>870</v>
       </c>
-      <c r="O57" s="169" t="s">
+      <c r="O57" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="P57" s="169"/>
+      <c r="P57" s="170"/>
     </row>
     <row r="58" spans="2:16">
       <c r="B58" s="28"/>
@@ -5946,10 +5968,10 @@
       </c>
     </row>
     <row r="59" spans="2:16" ht="23.25">
-      <c r="B59" s="187" t="s">
+      <c r="B59" s="196" t="s">
         <v>160</v>
       </c>
-      <c r="C59" s="187"/>
+      <c r="C59" s="196"/>
       <c r="N59" s="11"/>
       <c r="O59" s="42"/>
       <c r="P59" s="11"/>
@@ -6044,10 +6066,10 @@
       <c r="C69" s="12"/>
     </row>
     <row r="70" spans="2:3" ht="23.25">
-      <c r="B70" s="187" t="s">
+      <c r="B70" s="196" t="s">
         <v>161</v>
       </c>
-      <c r="C70" s="187"/>
+      <c r="C70" s="196"/>
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="13" t="s">
@@ -6070,10 +6092,10 @@
       <c r="C73" s="27"/>
     </row>
     <row r="74" spans="2:3" ht="23.25">
-      <c r="B74" s="188" t="s">
+      <c r="B74" s="197" t="s">
         <v>162</v>
       </c>
-      <c r="C74" s="188"/>
+      <c r="C74" s="197"/>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="13" t="s">
@@ -6136,10 +6158,10 @@
       <c r="C82" s="27"/>
     </row>
     <row r="83" spans="1:3" ht="18">
-      <c r="B83" s="189" t="s">
+      <c r="B83" s="198" t="s">
         <v>163</v>
       </c>
-      <c r="C83" s="189"/>
+      <c r="C83" s="198"/>
     </row>
     <row r="84" spans="1:3">
       <c r="B84" s="24" t="s">
@@ -6178,10 +6200,10 @@
       <c r="C88" s="31"/>
     </row>
     <row r="89" spans="1:3" ht="23.25">
-      <c r="B89" s="190" t="s">
+      <c r="B89" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="C89" s="190"/>
+      <c r="C89" s="199"/>
     </row>
     <row r="90" spans="1:3" ht="18.75">
       <c r="A90" s="139"/>
@@ -6256,14 +6278,14 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="B99" s="186" t="s">
+      <c r="B99" s="195" t="s">
         <v>272</v>
       </c>
-      <c r="C99" s="186"/>
+      <c r="C99" s="195"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="B100" s="186"/>
-      <c r="C100" s="186"/>
+      <c r="B100" s="195"/>
+      <c r="C100" s="195"/>
     </row>
     <row r="101" spans="1:3">
       <c r="B101" s="45" t="s">
@@ -6282,10 +6304,10 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="23.25">
-      <c r="B105" s="185" t="s">
+      <c r="B105" s="194" t="s">
         <v>285</v>
       </c>
-      <c r="C105" s="185"/>
+      <c r="C105" s="194"/>
     </row>
     <row r="106" spans="1:3" ht="18.75">
       <c r="B106" s="148" t="s">
@@ -6313,6 +6335,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B99:C100"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B89:C89"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="B1:G2"/>
@@ -6321,13 +6350,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B99:C100"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B89:C89"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B90" r:id="rId1" display="https://b2b.pramahikvision.com/goods/detail.html?goodsId=19672&amp;defaultViewProduct.productSapId=300611637&amp;selectType=all"/>
@@ -6370,22 +6392,22 @@
       <c r="E1" s="163"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
     </row>
     <row r="3" spans="1:6" ht="42" customHeight="1">
-      <c r="A3" s="175"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
+      <c r="A3" s="176"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="176"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="164"/>
@@ -6555,39 +6577,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="2:10" ht="69" customHeight="1">
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="2:10" ht="23.25">
-      <c r="B3" s="216" t="s">
+      <c r="B3" s="223" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="217"/>
-      <c r="H3" s="199" t="s">
+      <c r="C3" s="224"/>
+      <c r="H3" s="208" t="s">
         <v>346</v>
       </c>
-      <c r="I3" s="199"/>
-      <c r="J3" s="199"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="208"/>
     </row>
     <row r="4" spans="2:10" ht="23.25">
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="211" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="212"/>
       <c r="H4" s="45" t="s">
         <v>347</v>
       </c>
@@ -6627,10 +6649,10 @@
       <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:10" ht="26.25">
-      <c r="B7" s="206" t="s">
+      <c r="B7" s="213" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="206"/>
+      <c r="C7" s="213"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -6677,15 +6699,15 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="23.25">
-      <c r="B12" s="214" t="s">
+      <c r="B12" s="221" t="s">
         <v>254</v>
       </c>
-      <c r="C12" s="214"/>
-      <c r="H12" s="199" t="s">
+      <c r="C12" s="221"/>
+      <c r="H12" s="208" t="s">
         <v>357</v>
       </c>
-      <c r="I12" s="199"/>
-      <c r="J12" s="199"/>
+      <c r="I12" s="208"/>
+      <c r="J12" s="208"/>
     </row>
     <row r="13" spans="2:10" ht="18">
       <c r="B13" s="108" t="s">
@@ -6733,10 +6755,10 @@
       <c r="J15" s="17"/>
     </row>
     <row r="16" spans="2:10" ht="23.25">
-      <c r="B16" s="211" t="s">
+      <c r="B16" s="218" t="s">
         <v>255</v>
       </c>
-      <c r="C16" s="211"/>
+      <c r="C16" s="218"/>
       <c r="H16" s="45" t="s">
         <v>353</v>
       </c>
@@ -6776,15 +6798,15 @@
       <c r="C20" s="113"/>
     </row>
     <row r="21" spans="2:16" ht="23.25">
-      <c r="B21" s="215" t="s">
+      <c r="B21" s="222" t="s">
         <v>238</v>
       </c>
-      <c r="C21" s="215"/>
+      <c r="C21" s="222"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="169" t="s">
+      <c r="O21" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="P21" s="169"/>
+      <c r="P21" s="170"/>
     </row>
     <row r="22" spans="2:16" ht="18">
       <c r="B22" s="105" t="s">
@@ -6848,10 +6870,10 @@
       <c r="P26" s="11"/>
     </row>
     <row r="27" spans="2:16" ht="23.25">
-      <c r="B27" s="207" t="s">
+      <c r="B27" s="214" t="s">
         <v>241</v>
       </c>
-      <c r="C27" s="207"/>
+      <c r="C27" s="214"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
@@ -6924,10 +6946,10 @@
       <c r="C34" s="104"/>
     </row>
     <row r="35" spans="2:3" ht="23.25">
-      <c r="B35" s="212" t="s">
+      <c r="B35" s="219" t="s">
         <v>334</v>
       </c>
-      <c r="C35" s="213"/>
+      <c r="C35" s="220"/>
     </row>
     <row r="36" spans="2:3" ht="18">
       <c r="B36" s="107" t="s">
@@ -6946,10 +6968,10 @@
       </c>
     </row>
     <row r="38" spans="2:3" ht="23.25">
-      <c r="B38" s="208" t="s">
+      <c r="B38" s="215" t="s">
         <v>242</v>
       </c>
-      <c r="C38" s="209"/>
+      <c r="C38" s="216"/>
     </row>
     <row r="39" spans="2:3" ht="18.75">
       <c r="B39" s="115" t="s">
@@ -6968,10 +6990,10 @@
       </c>
     </row>
     <row r="41" spans="2:3" ht="18">
-      <c r="B41" s="202" t="s">
+      <c r="B41" s="209" t="s">
         <v>243</v>
       </c>
-      <c r="C41" s="203"/>
+      <c r="C41" s="210"/>
     </row>
     <row r="42" spans="2:3" ht="18">
       <c r="B42" s="107" t="s">
@@ -7094,10 +7116,10 @@
       <c r="C57" s="102"/>
     </row>
     <row r="58" spans="2:3" ht="23.25">
-      <c r="B58" s="204" t="s">
+      <c r="B58" s="211" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="205"/>
+      <c r="C58" s="212"/>
     </row>
     <row r="59" spans="2:3" ht="18.75">
       <c r="B59" s="118" t="s">
@@ -7152,10 +7174,10 @@
       </c>
     </row>
     <row r="66" spans="2:3" ht="26.25">
-      <c r="B66" s="218" t="s">
+      <c r="B66" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="219"/>
+      <c r="C66" s="201"/>
     </row>
     <row r="67" spans="2:3" ht="18.75">
       <c r="B67" s="115" t="s">
@@ -7202,10 +7224,10 @@
       <c r="C72" s="117"/>
     </row>
     <row r="73" spans="2:3" ht="26.25">
-      <c r="B73" s="218" t="s">
+      <c r="B73" s="200" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="219"/>
+      <c r="C73" s="201"/>
     </row>
     <row r="74" spans="2:3" ht="18.75">
       <c r="B74" s="119" t="s">
@@ -7268,10 +7290,10 @@
       <c r="C81" s="114"/>
     </row>
     <row r="82" spans="2:3" ht="28.5">
-      <c r="B82" s="210" t="s">
+      <c r="B82" s="217" t="s">
         <v>36</v>
       </c>
-      <c r="C82" s="210"/>
+      <c r="C82" s="217"/>
     </row>
     <row r="83" spans="2:3" ht="19.5" thickBot="1">
       <c r="B83" s="126" t="s">
@@ -7342,10 +7364,10 @@
       <c r="C91" s="114"/>
     </row>
     <row r="92" spans="2:3" ht="26.25">
-      <c r="B92" s="200" t="s">
+      <c r="B92" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="207"/>
     </row>
     <row r="93" spans="2:3" ht="18.75">
       <c r="B93" s="115" t="s">
@@ -7364,10 +7386,10 @@
       </c>
     </row>
     <row r="95" spans="2:3" ht="26.25">
-      <c r="B95" s="200" t="s">
+      <c r="B95" s="206" t="s">
         <v>146</v>
       </c>
-      <c r="C95" s="201"/>
+      <c r="C95" s="207"/>
     </row>
     <row r="96" spans="2:3" ht="18.75">
       <c r="B96" s="115" t="s">
@@ -7430,10 +7452,10 @@
       <c r="C103" s="102"/>
     </row>
     <row r="104" spans="2:3" ht="36">
-      <c r="B104" s="223" t="s">
+      <c r="B104" s="205" t="s">
         <v>166</v>
       </c>
-      <c r="C104" s="223"/>
+      <c r="C104" s="205"/>
     </row>
     <row r="105" spans="2:3" ht="23.25">
       <c r="B105" s="36" t="s">
@@ -7468,10 +7490,10 @@
       </c>
     </row>
     <row r="110" spans="2:3" ht="26.25">
-      <c r="B110" s="222" t="s">
+      <c r="B110" s="204" t="s">
         <v>277</v>
       </c>
-      <c r="C110" s="222"/>
+      <c r="C110" s="204"/>
     </row>
     <row r="111" spans="2:3" ht="23.25">
       <c r="B111" s="47" t="s">
@@ -7506,10 +7528,10 @@
       </c>
     </row>
     <row r="116" spans="2:3" ht="31.5">
-      <c r="B116" s="220" t="s">
+      <c r="B116" s="202" t="s">
         <v>427</v>
       </c>
-      <c r="C116" s="221"/>
+      <c r="C116" s="203"/>
     </row>
     <row r="117" spans="2:3" ht="21">
       <c r="B117" s="149" t="s">
@@ -7561,13 +7583,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H12:J12"/>
@@ -7584,6 +7599,13 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B73:C73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B75" r:id="rId1" display="https://b2b.pramahikvision.com/goods/detail.html?goodsId=20829&amp;defaultViewProduct.productSapId=301313364&amp;selectType=all"/>
@@ -7615,22 +7637,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
     </row>
     <row r="2" spans="1:20" ht="75" customHeight="1">
-      <c r="A2" s="175"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="A2" s="176"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
     </row>
     <row r="3" spans="1:20" ht="32.25" thickBot="1">
       <c r="A3" s="90" t="s">
@@ -7661,10 +7683,10 @@
       <c r="C5" s="152">
         <v>4200</v>
       </c>
-      <c r="F5" s="224">
+      <c r="F5" s="225">
         <v>76</v>
       </c>
-      <c r="H5" s="225">
+      <c r="H5" s="226">
         <v>76</v>
       </c>
     </row>
@@ -7678,8 +7700,8 @@
       <c r="C6" s="152">
         <v>4700</v>
       </c>
-      <c r="F6" s="224"/>
-      <c r="H6" s="225"/>
+      <c r="F6" s="225"/>
+      <c r="H6" s="226"/>
     </row>
     <row r="7" spans="1:20" ht="18">
       <c r="A7" s="150" t="s">
@@ -7691,8 +7713,8 @@
       <c r="C7" s="152">
         <v>5550</v>
       </c>
-      <c r="F7" s="224"/>
-      <c r="H7" s="225"/>
+      <c r="F7" s="225"/>
+      <c r="H7" s="226"/>
     </row>
     <row r="8" spans="1:20" ht="18">
       <c r="A8" s="150" t="s">
@@ -7704,8 +7726,8 @@
       <c r="C8" s="153">
         <v>5700</v>
       </c>
-      <c r="F8" s="224"/>
-      <c r="H8" s="225"/>
+      <c r="F8" s="225"/>
+      <c r="H8" s="226"/>
     </row>
     <row r="9" spans="1:20" ht="18">
       <c r="A9" s="150" t="s">
@@ -7717,8 +7739,8 @@
       <c r="C9" s="153">
         <v>6750</v>
       </c>
-      <c r="F9" s="224"/>
-      <c r="H9" s="225"/>
+      <c r="F9" s="225"/>
+      <c r="H9" s="226"/>
     </row>
     <row r="10" spans="1:20" ht="18">
       <c r="A10" s="87" t="s">
@@ -7728,8 +7750,8 @@
       <c r="C10" s="89">
         <v>11900</v>
       </c>
-      <c r="F10" s="224"/>
-      <c r="H10" s="225"/>
+      <c r="F10" s="225"/>
+      <c r="H10" s="226"/>
     </row>
     <row r="11" spans="1:20" ht="18">
       <c r="A11" s="150" t="s">
@@ -7741,8 +7763,8 @@
       <c r="C11" s="153">
         <v>6300</v>
       </c>
-      <c r="F11" s="224"/>
-      <c r="H11" s="225"/>
+      <c r="F11" s="225"/>
+      <c r="H11" s="226"/>
     </row>
     <row r="12" spans="1:20" ht="18">
       <c r="A12" s="150" t="s">
@@ -7754,8 +7776,8 @@
       <c r="C12" s="153">
         <v>9350</v>
       </c>
-      <c r="F12" s="224"/>
-      <c r="H12" s="225"/>
+      <c r="F12" s="225"/>
+      <c r="H12" s="226"/>
     </row>
     <row r="13" spans="1:20" ht="18">
       <c r="A13" s="150" t="s">
@@ -7779,10 +7801,10 @@
         <v>14500</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="169" t="s">
+      <c r="S14" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="T14" s="169"/>
+      <c r="T14" s="170"/>
     </row>
     <row r="15" spans="1:20" ht="18">
       <c r="A15" s="150" t="s">
@@ -7913,10 +7935,10 @@
       <c r="C27" s="156">
         <v>5250</v>
       </c>
-      <c r="F27" s="225">
+      <c r="F27" s="226">
         <v>76</v>
       </c>
-      <c r="H27" s="225">
+      <c r="H27" s="226">
         <v>76</v>
       </c>
     </row>
@@ -7928,8 +7950,8 @@
       <c r="C28" s="156">
         <v>7200</v>
       </c>
-      <c r="F28" s="225"/>
-      <c r="H28" s="225"/>
+      <c r="F28" s="226"/>
+      <c r="H28" s="226"/>
     </row>
     <row r="29" spans="1:20" ht="18">
       <c r="A29" s="157" t="s">
@@ -7939,8 +7961,8 @@
       <c r="C29" s="156">
         <v>8750</v>
       </c>
-      <c r="F29" s="225"/>
-      <c r="H29" s="225"/>
+      <c r="F29" s="226"/>
+      <c r="H29" s="226"/>
     </row>
     <row r="30" spans="1:20" ht="18">
       <c r="A30" s="157" t="s">
@@ -7950,8 +7972,8 @@
       <c r="C30" s="156">
         <v>7400</v>
       </c>
-      <c r="F30" s="225"/>
-      <c r="H30" s="225"/>
+      <c r="F30" s="226"/>
+      <c r="H30" s="226"/>
     </row>
     <row r="31" spans="1:20" ht="18">
       <c r="A31" s="157" t="s">
@@ -7961,8 +7983,8 @@
       <c r="C31" s="156">
         <v>11300</v>
       </c>
-      <c r="F31" s="225"/>
-      <c r="H31" s="225"/>
+      <c r="F31" s="226"/>
+      <c r="H31" s="226"/>
     </row>
     <row r="32" spans="1:20" ht="18">
       <c r="A32" s="157" t="s">
@@ -7972,8 +7994,8 @@
       <c r="C32" s="156">
         <v>16900</v>
       </c>
-      <c r="F32" s="225"/>
-      <c r="H32" s="225"/>
+      <c r="F32" s="226"/>
+      <c r="H32" s="226"/>
     </row>
     <row r="33" spans="1:6" ht="18">
       <c r="A33" s="157" t="s">
@@ -8217,11 +8239,11 @@
       </c>
     </row>
     <row r="18" spans="4:6" ht="21">
-      <c r="D18" s="226" t="s">
+      <c r="D18" s="227" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="226"/>
-      <c r="F18" s="226"/>
+      <c r="E18" s="227"/>
+      <c r="F18" s="227"/>
     </row>
     <row r="19" spans="4:6" ht="21">
       <c r="D19" s="21" t="s">
@@ -8260,11 +8282,11 @@
       </c>
     </row>
     <row r="23" spans="4:6" ht="21">
-      <c r="D23" s="227" t="s">
+      <c r="D23" s="228" t="s">
         <v>164</v>
       </c>
-      <c r="E23" s="228"/>
-      <c r="F23" s="229"/>
+      <c r="E23" s="229"/>
+      <c r="F23" s="230"/>
     </row>
     <row r="24" spans="4:6" ht="21">
       <c r="D24" s="21" t="s">
@@ -8406,30 +8428,30 @@
   <sheetData>
     <row r="1" spans="6:12" hidden="1"/>
     <row r="2" spans="6:12">
-      <c r="G2" s="230" t="s">
+      <c r="G2" s="231" t="s">
         <v>432</v>
       </c>
-      <c r="H2" s="231"/>
-      <c r="I2" s="231"/>
-      <c r="J2" s="231"/>
-      <c r="K2" s="231"/>
-      <c r="L2" s="231"/>
+      <c r="H2" s="232"/>
+      <c r="I2" s="232"/>
+      <c r="J2" s="232"/>
+      <c r="K2" s="232"/>
+      <c r="L2" s="232"/>
     </row>
     <row r="3" spans="6:12" ht="52.5" customHeight="1">
-      <c r="G3" s="231"/>
-      <c r="H3" s="231"/>
-      <c r="I3" s="231"/>
-      <c r="J3" s="231"/>
-      <c r="K3" s="231"/>
-      <c r="L3" s="231"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="232"/>
+      <c r="I3" s="232"/>
+      <c r="J3" s="232"/>
+      <c r="K3" s="232"/>
+      <c r="L3" s="232"/>
     </row>
     <row r="5" spans="6:12" ht="18">
-      <c r="F5" s="233" t="s">
+      <c r="F5" s="234" t="s">
         <v>197</v>
       </c>
-      <c r="G5" s="234"/>
-      <c r="H5" s="234"/>
-      <c r="I5" s="234"/>
+      <c r="G5" s="235"/>
+      <c r="H5" s="235"/>
+      <c r="I5" s="235"/>
     </row>
     <row r="6" spans="6:12" ht="63">
       <c r="F6" s="48" t="s">
@@ -8452,13 +8474,13 @@
       <c r="F7" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="235" t="s">
+      <c r="G7" s="236" t="s">
         <v>142</v>
       </c>
       <c r="H7" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="I7" s="236" t="s">
+      <c r="I7" s="237" t="s">
         <v>202</v>
       </c>
       <c r="J7" s="54">
@@ -8469,11 +8491,11 @@
       <c r="F8" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="G8" s="235"/>
+      <c r="G8" s="236"/>
       <c r="H8" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="I8" s="236"/>
+      <c r="I8" s="237"/>
       <c r="J8" s="54">
         <v>1993.95</v>
       </c>
@@ -8576,7 +8598,7 @@
       <c r="H15" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="I15" s="237" t="s">
+      <c r="I15" s="238" t="s">
         <v>296</v>
       </c>
       <c r="J15" s="68">
@@ -8591,7 +8613,7 @@
       <c r="H16" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="I16" s="238"/>
+      <c r="I16" s="239"/>
       <c r="J16" s="68">
         <v>3849.3</v>
       </c>
@@ -8600,11 +8622,11 @@
       <c r="F17" s="69" t="s">
         <v>217</v>
       </c>
-      <c r="G17" s="239"/>
+      <c r="G17" s="240"/>
       <c r="H17" s="70" t="s">
         <v>218</v>
       </c>
-      <c r="I17" s="232" t="s">
+      <c r="I17" s="233" t="s">
         <v>219</v>
       </c>
       <c r="J17" s="71">
@@ -8615,11 +8637,11 @@
       <c r="F18" s="69" t="s">
         <v>220</v>
       </c>
-      <c r="G18" s="239"/>
+      <c r="G18" s="240"/>
       <c r="H18" s="70" t="s">
         <v>221</v>
       </c>
-      <c r="I18" s="232"/>
+      <c r="I18" s="233"/>
       <c r="J18" s="71">
         <v>4141.2</v>
       </c>
@@ -8705,11 +8727,11 @@
       </c>
     </row>
     <row r="4" spans="4:6" ht="26.25">
-      <c r="D4" s="241" t="s">
+      <c r="D4" s="242" t="s">
         <v>333</v>
       </c>
-      <c r="E4" s="241"/>
-      <c r="F4" s="241"/>
+      <c r="E4" s="242"/>
+      <c r="F4" s="242"/>
     </row>
     <row r="5" spans="4:6" ht="23.25">
       <c r="D5" s="16" t="s">
@@ -8794,11 +8816,11 @@
       <c r="F12" s="17"/>
     </row>
     <row r="18" spans="4:6" ht="31.5">
-      <c r="D18" s="240" t="s">
+      <c r="D18" s="241" t="s">
         <v>332</v>
       </c>
-      <c r="E18" s="240"/>
-      <c r="F18" s="240"/>
+      <c r="E18" s="241"/>
+      <c r="F18" s="241"/>
     </row>
     <row r="19" spans="4:6" ht="23.25">
       <c r="D19" s="16" t="s">
@@ -8858,7 +8880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -8875,7 +8897,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75">
-      <c r="B3" s="242" t="s">
+      <c r="B3" s="169" t="s">
         <v>436</v>
       </c>
     </row>
@@ -8885,7 +8907,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="169" t="s">
         <v>437</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Hikvision file has been updated"
This reverts commit 68a27b0a20e85fc11d12537ac670c956b25ff9f7.
</commit_message>
<xml_diff>
--- a/HIKVISION JUNE 2021 PRICE LIST (MOP).xlsx
+++ b/HIKVISION JUNE 2021 PRICE LIST (MOP).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meljo scans\AWS related\DEvOps 1\DEVOPSGITTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\easo mathew\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="HD DVR" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="EZVIZ" sheetId="7" r:id="rId7"/>
     <sheet name="BIOMETRIC" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="440">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1431,9 +1430,6 @@
   </si>
   <si>
     <t>CAMERA</t>
-  </si>
-  <si>
-    <t>Hello this is a test file updation. Git is here.</t>
   </si>
 </sst>
 </file>
@@ -2880,7 +2876,6 @@
     <xf numFmtId="0" fontId="92" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2929,6 +2924,24 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2953,22 +2966,61 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2989,63 +3041,6 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3100,6 +3095,7 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3139,7 +3135,7 @@
         <xdr:cNvPr id="2757" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F794545B-F0AD-4D5E-A9B7-5F7DD3D743EA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F794545B-F0AD-4D5E-A9B7-5F7DD3D743EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3213,7 +3209,7 @@
         <xdr:cNvPr id="2758" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15D3C60F-939C-4EB5-9518-224E25F16960}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D3C60F-939C-4EB5-9518-224E25F16960}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3292,7 +3288,7 @@
         <xdr:cNvPr id="14564" name="Picture 10" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F450D326-A10A-4C17-932A-29E325E7772B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F450D326-A10A-4C17-932A-29E325E7772B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3366,7 +3362,7 @@
         <xdr:cNvPr id="14565" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B7163B-A39D-4579-BF37-31F72DF3A3E1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B7163B-A39D-4579-BF37-31F72DF3A3E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3440,7 +3436,7 @@
         <xdr:cNvPr id="14566" name="Picture 12" descr="Image result for CS-X5C-4APEC">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEF73321-D25C-4263-A062-A8A4A50B64A6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEF73321-D25C-4263-A062-A8A4A50B64A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3514,7 +3510,7 @@
         <xdr:cNvPr id="14567" name="Picture 13" descr="Image result for C1C CAMERA">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4FABD93E-A38C-433B-ACE6-ABABF15DE2DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FABD93E-A38C-433B-ACE6-ABABF15DE2DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3588,7 +3584,7 @@
         <xdr:cNvPr id="14568" name="Picture 14" descr="Image result for CS-CV346-AO-7A3WFR(3MP)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{77CFCDF6-B04D-4EC4-AC5D-ED82A54AB919}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77CFCDF6-B04D-4EC4-AC5D-ED82A54AB919}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3662,7 +3658,7 @@
         <xdr:cNvPr id="14569" name="Picture 15" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A2F14B0F-DD82-40C8-B42B-F711EB4B66F8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F14B0F-DD82-40C8-B42B-F711EB4B66F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3736,7 +3732,7 @@
         <xdr:cNvPr id="14570" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A45B85A1-918B-48CB-9D61-7AB33CABEF38}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45B85A1-918B-48CB-9D61-7AB33CABEF38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3810,7 +3806,7 @@
         <xdr:cNvPr id="14571" name="Picture 15" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6B0AD6D-C36D-4E0A-81DD-DF43FC954379}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6B0AD6D-C36D-4E0A-81DD-DF43FC954379}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3884,7 +3880,7 @@
         <xdr:cNvPr id="14572" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB2C1C4E-39B8-419D-8C58-48DCE0C63BA0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2C1C4E-39B8-419D-8C58-48DCE0C63BA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3958,7 +3954,7 @@
         <xdr:cNvPr id="14573" name="AutoShape 3" descr="Image result for CS-CV310-A0-1B2WFR">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{58FE2307-73C2-4B94-A8A4-6F0CE4F0ACFF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58FE2307-73C2-4B94-A8A4-6F0CE4F0ACFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4019,7 +4015,7 @@
         <xdr:cNvPr id="14574" name="Picture 13" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B7080737-A6C9-4FBB-B8A4-29BA5D8D30DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7080737-A6C9-4FBB-B8A4-29BA5D8D30DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4093,7 +4089,7 @@
         <xdr:cNvPr id="14575" name="Picture 15" descr="Image result for C1C CAMERA">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E0B5B8F1-63F4-4958-B1D3-30B9BA7F7815}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0B5B8F1-63F4-4958-B1D3-30B9BA7F7815}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4167,7 +4163,7 @@
         <xdr:cNvPr id="14576" name="Picture 16" descr="Image result for CS-CV346-AO-7A3WFR(3MP)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CF2ED700-160A-4191-A9B9-F382F2F9E451}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2ED700-160A-4191-A9B9-F382F2F9E451}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4241,7 +4237,7 @@
         <xdr:cNvPr id="14577" name="Picture 17" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBFB5773-8A75-4665-AC47-44CC01BB972B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBFB5773-8A75-4665-AC47-44CC01BB972B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4315,7 +4311,7 @@
         <xdr:cNvPr id="14578" name="Picture 18" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E035C21-C91C-4651-B4FD-A1ECA30E860D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E035C21-C91C-4651-B4FD-A1ECA30E860D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4389,7 +4385,7 @@
         <xdr:cNvPr id="14579" name="Picture 19" descr="Image result for EZVIZ NVR KIT">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{397FF8EE-BFB2-4FE7-A3B2-F9942321552C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397FF8EE-BFB2-4FE7-A3B2-F9942321552C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4463,7 +4459,7 @@
         <xdr:cNvPr id="14580" name="Picture 20" descr="Camera IP EZVIZ CS-C3N (A0-3H2WFRL) 1080P Có Màu Ban Đêm - Hàng ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B46A902-DED4-4EA9-A473-659B44C1B7AC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B46A902-DED4-4EA9-A473-659B44C1B7AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4537,7 +4533,7 @@
         <xdr:cNvPr id="14581" name="Picture 21" descr="Camera IP EZVIZ CS-C3N (A0-3H2WFRL) 1080P Có Màu Ban Đêm - Hàng ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{691C9B81-B5BB-4F80-A630-EAF4F98C6EB0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691C9B81-B5BB-4F80-A630-EAF4F98C6EB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4611,7 +4607,7 @@
         <xdr:cNvPr id="14582" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7354854F-34EB-4903-A01B-7844B435C044}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7354854F-34EB-4903-A01B-7844B435C044}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4977,22 +4973,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="174" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
     </row>
     <row r="2" spans="2:17" ht="86.25" customHeight="1">
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="32" t="s">
@@ -5004,10 +5000,10 @@
       <c r="F3" s="41"/>
     </row>
     <row r="4" spans="2:17" ht="23.25">
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="179" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="181"/>
+      <c r="C4" s="180"/>
     </row>
     <row r="5" spans="2:17" ht="15.75">
       <c r="B5" s="128" t="s">
@@ -5016,7 +5012,7 @@
       <c r="C5" s="84">
         <v>2900</v>
       </c>
-      <c r="G5" s="178"/>
+      <c r="G5" s="177"/>
     </row>
     <row r="6" spans="2:17" ht="15.75">
       <c r="B6" s="128" t="s">
@@ -5025,11 +5021,11 @@
       <c r="C6" s="84">
         <v>4340</v>
       </c>
-      <c r="G6" s="178"/>
-      <c r="P6" s="170" t="s">
+      <c r="G6" s="177"/>
+      <c r="P6" s="169" t="s">
         <v>180</v>
       </c>
-      <c r="Q6" s="170"/>
+      <c r="Q6" s="169"/>
     </row>
     <row r="7" spans="2:17" ht="15.75">
       <c r="B7" s="128" t="s">
@@ -5038,7 +5034,7 @@
       <c r="C7" s="84">
         <v>7550</v>
       </c>
-      <c r="G7" s="178"/>
+      <c r="G7" s="177"/>
       <c r="O7" s="11" t="s">
         <v>39</v>
       </c>
@@ -5050,10 +5046,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" ht="23.25">
-      <c r="B8" s="182" t="s">
+      <c r="B8" s="181" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="183"/>
+      <c r="C8" s="182"/>
       <c r="G8" s="25"/>
       <c r="O8" s="11"/>
       <c r="P8" s="42"/>
@@ -5066,7 +5062,7 @@
       <c r="C9" s="130">
         <v>2350</v>
       </c>
-      <c r="G9" s="179" t="s">
+      <c r="G9" s="178" t="s">
         <v>66</v>
       </c>
       <c r="O9" s="11"/>
@@ -5080,7 +5076,7 @@
       <c r="C10" s="130">
         <v>3550</v>
       </c>
-      <c r="G10" s="179"/>
+      <c r="G10" s="178"/>
       <c r="O10" s="11"/>
       <c r="P10" s="42"/>
       <c r="Q10" s="11"/>
@@ -5092,7 +5088,7 @@
       <c r="C11" s="130">
         <v>5950</v>
       </c>
-      <c r="G11" s="179"/>
+      <c r="G11" s="178"/>
       <c r="O11" s="11"/>
       <c r="P11" s="42"/>
       <c r="Q11" s="11"/>
@@ -5104,7 +5100,7 @@
       <c r="C12" s="130">
         <v>5950</v>
       </c>
-      <c r="G12" s="179"/>
+      <c r="G12" s="178"/>
       <c r="O12" s="11"/>
       <c r="P12" s="42"/>
       <c r="Q12" s="11"/>
@@ -5116,7 +5112,7 @@
       <c r="C13" s="130">
         <v>8200</v>
       </c>
-      <c r="G13" s="179"/>
+      <c r="G13" s="178"/>
       <c r="O13" s="11"/>
       <c r="P13" s="42"/>
       <c r="Q13" s="11"/>
@@ -5128,17 +5124,17 @@
       <c r="C14" s="130">
         <v>17500</v>
       </c>
-      <c r="G14" s="179"/>
+      <c r="G14" s="178"/>
       <c r="O14" s="43"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="43"/>
     </row>
     <row r="15" spans="2:17" ht="23.25">
-      <c r="B15" s="182" t="s">
+      <c r="B15" s="181" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="183"/>
-      <c r="G15" s="179"/>
+      <c r="C15" s="182"/>
+      <c r="G15" s="178"/>
       <c r="P15" s="41"/>
     </row>
     <row r="16" spans="2:17" ht="15.75">
@@ -5148,7 +5144,7 @@
       <c r="C16" s="130">
         <v>10500</v>
       </c>
-      <c r="G16" s="179"/>
+      <c r="G16" s="178"/>
       <c r="P16" s="41"/>
     </row>
     <row r="17" spans="2:16" ht="15.75">
@@ -5158,7 +5154,7 @@
       <c r="C17" s="130">
         <v>14500</v>
       </c>
-      <c r="G17" s="179"/>
+      <c r="G17" s="178"/>
       <c r="P17" s="41"/>
     </row>
     <row r="18" spans="2:16" ht="15.75">
@@ -5168,7 +5164,7 @@
       <c r="C18" s="130">
         <v>3900</v>
       </c>
-      <c r="G18" s="179"/>
+      <c r="G18" s="178"/>
       <c r="P18" s="41"/>
     </row>
     <row r="19" spans="2:16" ht="15.75">
@@ -5178,7 +5174,7 @@
       <c r="C19" s="130">
         <v>5720</v>
       </c>
-      <c r="G19" s="179"/>
+      <c r="G19" s="178"/>
       <c r="P19" s="41"/>
     </row>
     <row r="20" spans="2:16" ht="15.75">
@@ -5188,7 +5184,7 @@
       <c r="C20" s="130">
         <v>9800</v>
       </c>
-      <c r="G20" s="179"/>
+      <c r="G20" s="178"/>
       <c r="P20" s="41"/>
     </row>
     <row r="21" spans="2:16" ht="15.75">
@@ -5198,7 +5194,7 @@
       <c r="C21" s="130">
         <v>7900</v>
       </c>
-      <c r="G21" s="179"/>
+      <c r="G21" s="178"/>
       <c r="P21" s="41"/>
     </row>
     <row r="22" spans="2:16" ht="15.75">
@@ -5208,15 +5204,15 @@
       <c r="C22" s="130">
         <v>11500</v>
       </c>
-      <c r="G22" s="179"/>
+      <c r="G22" s="178"/>
       <c r="P22" s="41"/>
     </row>
     <row r="23" spans="2:16" ht="20.25">
-      <c r="B23" s="184" t="s">
+      <c r="B23" s="183" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="185"/>
-      <c r="G23" s="179"/>
+      <c r="C23" s="184"/>
+      <c r="G23" s="178"/>
       <c r="P23" s="41"/>
     </row>
     <row r="24" spans="2:16" ht="15.75">
@@ -5226,7 +5222,7 @@
       <c r="C24" s="84" t="s">
         <v>384</v>
       </c>
-      <c r="G24" s="179"/>
+      <c r="G24" s="178"/>
       <c r="P24" s="41"/>
     </row>
     <row r="25" spans="2:16" ht="15.75">
@@ -5236,7 +5232,7 @@
       <c r="C25" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="G25" s="179"/>
+      <c r="G25" s="178"/>
       <c r="P25" s="41"/>
     </row>
     <row r="26" spans="2:16" ht="15.75">
@@ -5246,7 +5242,7 @@
       <c r="C26" s="84">
         <v>0</v>
       </c>
-      <c r="G26" s="179"/>
+      <c r="G26" s="178"/>
       <c r="P26" s="41"/>
     </row>
     <row r="27" spans="2:16" ht="15.75">
@@ -5256,7 +5252,7 @@
       <c r="C27" s="84" t="s">
         <v>386</v>
       </c>
-      <c r="G27" s="179"/>
+      <c r="G27" s="178"/>
       <c r="P27" s="41"/>
     </row>
     <row r="28" spans="2:16" ht="15.75">
@@ -5266,7 +5262,7 @@
       <c r="C28" s="84">
         <v>17000</v>
       </c>
-      <c r="G28" s="179"/>
+      <c r="G28" s="178"/>
     </row>
     <row r="29" spans="2:16" ht="15.75">
       <c r="B29" s="128" t="s">
@@ -5278,10 +5274,10 @@
       <c r="G29" s="40"/>
     </row>
     <row r="30" spans="2:16" ht="26.25">
-      <c r="B30" s="173" t="s">
+      <c r="B30" s="172" t="s">
         <v>276</v>
       </c>
-      <c r="C30" s="174"/>
+      <c r="C30" s="173"/>
     </row>
     <row r="31" spans="2:16" ht="15.75">
       <c r="B31" s="131" t="s">
@@ -5300,10 +5296,10 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="20.25">
-      <c r="B35" s="177" t="s">
+      <c r="B35" s="176" t="s">
         <v>152</v>
       </c>
-      <c r="C35" s="177"/>
+      <c r="C35" s="176"/>
     </row>
     <row r="36" spans="2:4" ht="15.75">
       <c r="B36" s="86" t="s">
@@ -5334,10 +5330,10 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="20.25">
-      <c r="B40" s="171" t="s">
+      <c r="B40" s="170" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="171"/>
+      <c r="C40" s="170"/>
     </row>
     <row r="41" spans="2:4" ht="15.75">
       <c r="B41" s="131" t="s">
@@ -5362,10 +5358,10 @@
       <c r="C43" s="132"/>
     </row>
     <row r="45" spans="2:4" ht="18">
-      <c r="B45" s="172" t="s">
+      <c r="B45" s="171" t="s">
         <v>154</v>
       </c>
-      <c r="C45" s="172"/>
+      <c r="C45" s="171"/>
     </row>
     <row r="46" spans="2:4" ht="15.75">
       <c r="B46" s="131" t="s">
@@ -5416,24 +5412,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5459,39 +5437,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="174" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
     </row>
     <row r="2" spans="2:10" ht="87.75" customHeight="1">
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="3" spans="2:10" ht="15.75">
       <c r="B3" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="35"/>
-      <c r="H3" s="186" t="s">
+      <c r="H3" s="191" t="s">
         <v>431</v>
       </c>
-      <c r="I3" s="186"/>
-      <c r="J3" s="186"/>
+      <c r="I3" s="191"/>
+      <c r="J3" s="191"/>
     </row>
     <row r="4" spans="2:10" ht="26.25">
-      <c r="B4" s="189" t="s">
+      <c r="B4" s="194" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="190"/>
+      <c r="C4" s="195"/>
       <c r="H4" s="45" t="s">
         <v>337</v>
       </c>
@@ -5559,11 +5537,11 @@
       <c r="C9" s="130">
         <v>1600</v>
       </c>
-      <c r="H9" s="187" t="s">
+      <c r="H9" s="192" t="s">
         <v>341</v>
       </c>
-      <c r="I9" s="187"/>
-      <c r="J9" s="187"/>
+      <c r="I9" s="192"/>
+      <c r="J9" s="192"/>
     </row>
     <row r="10" spans="2:10" ht="30">
       <c r="B10" s="141" t="s">
@@ -5641,10 +5619,10 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="27">
-      <c r="B16" s="191" t="s">
+      <c r="B16" s="196" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="192"/>
+      <c r="C16" s="197"/>
     </row>
     <row r="17" spans="2:3" ht="17.25">
       <c r="B17" s="142" t="s">
@@ -5795,10 +5773,10 @@
       <c r="C35" s="12"/>
     </row>
     <row r="36" spans="2:3" ht="20.25">
-      <c r="B36" s="193" t="s">
+      <c r="B36" s="198" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="193"/>
+      <c r="C36" s="198"/>
     </row>
     <row r="37" spans="2:3" ht="15.75">
       <c r="B37" s="146" t="s">
@@ -5897,10 +5875,10 @@
       <c r="C49" s="1"/>
     </row>
     <row r="51" spans="2:16" ht="23.25">
-      <c r="B51" s="188" t="s">
+      <c r="B51" s="193" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="188"/>
+      <c r="C51" s="193"/>
     </row>
     <row r="52" spans="2:16" ht="17.25">
       <c r="B52" s="141" t="s">
@@ -5949,10 +5927,10 @@
       <c r="C57" s="140">
         <v>870</v>
       </c>
-      <c r="O57" s="170" t="s">
+      <c r="O57" s="169" t="s">
         <v>180</v>
       </c>
-      <c r="P57" s="170"/>
+      <c r="P57" s="169"/>
     </row>
     <row r="58" spans="2:16">
       <c r="B58" s="28"/>
@@ -5968,10 +5946,10 @@
       </c>
     </row>
     <row r="59" spans="2:16" ht="23.25">
-      <c r="B59" s="196" t="s">
+      <c r="B59" s="187" t="s">
         <v>160</v>
       </c>
-      <c r="C59" s="196"/>
+      <c r="C59" s="187"/>
       <c r="N59" s="11"/>
       <c r="O59" s="42"/>
       <c r="P59" s="11"/>
@@ -6066,10 +6044,10 @@
       <c r="C69" s="12"/>
     </row>
     <row r="70" spans="2:3" ht="23.25">
-      <c r="B70" s="196" t="s">
+      <c r="B70" s="187" t="s">
         <v>161</v>
       </c>
-      <c r="C70" s="196"/>
+      <c r="C70" s="187"/>
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="13" t="s">
@@ -6092,10 +6070,10 @@
       <c r="C73" s="27"/>
     </row>
     <row r="74" spans="2:3" ht="23.25">
-      <c r="B74" s="197" t="s">
+      <c r="B74" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="C74" s="197"/>
+      <c r="C74" s="188"/>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="13" t="s">
@@ -6158,10 +6136,10 @@
       <c r="C82" s="27"/>
     </row>
     <row r="83" spans="1:3" ht="18">
-      <c r="B83" s="198" t="s">
+      <c r="B83" s="189" t="s">
         <v>163</v>
       </c>
-      <c r="C83" s="198"/>
+      <c r="C83" s="189"/>
     </row>
     <row r="84" spans="1:3">
       <c r="B84" s="24" t="s">
@@ -6200,10 +6178,10 @@
       <c r="C88" s="31"/>
     </row>
     <row r="89" spans="1:3" ht="23.25">
-      <c r="B89" s="199" t="s">
+      <c r="B89" s="190" t="s">
         <v>271</v>
       </c>
-      <c r="C89" s="199"/>
+      <c r="C89" s="190"/>
     </row>
     <row r="90" spans="1:3" ht="18.75">
       <c r="A90" s="139"/>
@@ -6278,14 +6256,14 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="B99" s="195" t="s">
+      <c r="B99" s="186" t="s">
         <v>272</v>
       </c>
-      <c r="C99" s="195"/>
+      <c r="C99" s="186"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="B100" s="195"/>
-      <c r="C100" s="195"/>
+      <c r="B100" s="186"/>
+      <c r="C100" s="186"/>
     </row>
     <row r="101" spans="1:3">
       <c r="B101" s="45" t="s">
@@ -6304,10 +6282,10 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="23.25">
-      <c r="B105" s="194" t="s">
+      <c r="B105" s="185" t="s">
         <v>285</v>
       </c>
-      <c r="C105" s="194"/>
+      <c r="C105" s="185"/>
     </row>
     <row r="106" spans="1:3" ht="18.75">
       <c r="B106" s="148" t="s">
@@ -6335,13 +6313,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B99:C100"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B89:C89"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="B1:G2"/>
@@ -6350,6 +6321,13 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B99:C100"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B89:C89"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B90" r:id="rId1" display="https://b2b.pramahikvision.com/goods/detail.html?goodsId=19672&amp;defaultViewProduct.productSapId=300611637&amp;selectType=all"/>
@@ -6392,22 +6370,22 @@
       <c r="E1" s="163"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="174" t="s">
         <v>432</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
     </row>
     <row r="3" spans="1:6" ht="42" customHeight="1">
-      <c r="A3" s="176"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
+      <c r="A3" s="175"/>
+      <c r="B3" s="175"/>
+      <c r="C3" s="175"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
+      <c r="F3" s="175"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="164"/>
@@ -6577,39 +6555,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="174" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
     </row>
     <row r="2" spans="2:10" ht="69" customHeight="1">
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
     </row>
     <row r="3" spans="2:10" ht="23.25">
-      <c r="B3" s="223" t="s">
+      <c r="B3" s="216" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="H3" s="208" t="s">
+      <c r="C3" s="217"/>
+      <c r="H3" s="199" t="s">
         <v>346</v>
       </c>
-      <c r="I3" s="208"/>
-      <c r="J3" s="208"/>
+      <c r="I3" s="199"/>
+      <c r="J3" s="199"/>
     </row>
     <row r="4" spans="2:10" ht="23.25">
-      <c r="B4" s="211" t="s">
+      <c r="B4" s="204" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="212"/>
+      <c r="C4" s="205"/>
       <c r="H4" s="45" t="s">
         <v>347</v>
       </c>
@@ -6649,10 +6627,10 @@
       <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:10" ht="26.25">
-      <c r="B7" s="213" t="s">
+      <c r="B7" s="206" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="213"/>
+      <c r="C7" s="206"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -6699,15 +6677,15 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="23.25">
-      <c r="B12" s="221" t="s">
+      <c r="B12" s="214" t="s">
         <v>254</v>
       </c>
-      <c r="C12" s="221"/>
-      <c r="H12" s="208" t="s">
+      <c r="C12" s="214"/>
+      <c r="H12" s="199" t="s">
         <v>357</v>
       </c>
-      <c r="I12" s="208"/>
-      <c r="J12" s="208"/>
+      <c r="I12" s="199"/>
+      <c r="J12" s="199"/>
     </row>
     <row r="13" spans="2:10" ht="18">
       <c r="B13" s="108" t="s">
@@ -6755,10 +6733,10 @@
       <c r="J15" s="17"/>
     </row>
     <row r="16" spans="2:10" ht="23.25">
-      <c r="B16" s="218" t="s">
+      <c r="B16" s="211" t="s">
         <v>255</v>
       </c>
-      <c r="C16" s="218"/>
+      <c r="C16" s="211"/>
       <c r="H16" s="45" t="s">
         <v>353</v>
       </c>
@@ -6798,15 +6776,15 @@
       <c r="C20" s="113"/>
     </row>
     <row r="21" spans="2:16" ht="23.25">
-      <c r="B21" s="222" t="s">
+      <c r="B21" s="215" t="s">
         <v>238</v>
       </c>
-      <c r="C21" s="222"/>
+      <c r="C21" s="215"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="170" t="s">
+      <c r="O21" s="169" t="s">
         <v>180</v>
       </c>
-      <c r="P21" s="170"/>
+      <c r="P21" s="169"/>
     </row>
     <row r="22" spans="2:16" ht="18">
       <c r="B22" s="105" t="s">
@@ -6870,10 +6848,10 @@
       <c r="P26" s="11"/>
     </row>
     <row r="27" spans="2:16" ht="23.25">
-      <c r="B27" s="214" t="s">
+      <c r="B27" s="207" t="s">
         <v>241</v>
       </c>
-      <c r="C27" s="214"/>
+      <c r="C27" s="207"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
@@ -6946,10 +6924,10 @@
       <c r="C34" s="104"/>
     </row>
     <row r="35" spans="2:3" ht="23.25">
-      <c r="B35" s="219" t="s">
+      <c r="B35" s="212" t="s">
         <v>334</v>
       </c>
-      <c r="C35" s="220"/>
+      <c r="C35" s="213"/>
     </row>
     <row r="36" spans="2:3" ht="18">
       <c r="B36" s="107" t="s">
@@ -6968,10 +6946,10 @@
       </c>
     </row>
     <row r="38" spans="2:3" ht="23.25">
-      <c r="B38" s="215" t="s">
+      <c r="B38" s="208" t="s">
         <v>242</v>
       </c>
-      <c r="C38" s="216"/>
+      <c r="C38" s="209"/>
     </row>
     <row r="39" spans="2:3" ht="18.75">
       <c r="B39" s="115" t="s">
@@ -6990,10 +6968,10 @@
       </c>
     </row>
     <row r="41" spans="2:3" ht="18">
-      <c r="B41" s="209" t="s">
+      <c r="B41" s="202" t="s">
         <v>243</v>
       </c>
-      <c r="C41" s="210"/>
+      <c r="C41" s="203"/>
     </row>
     <row r="42" spans="2:3" ht="18">
       <c r="B42" s="107" t="s">
@@ -7116,10 +7094,10 @@
       <c r="C57" s="102"/>
     </row>
     <row r="58" spans="2:3" ht="23.25">
-      <c r="B58" s="211" t="s">
+      <c r="B58" s="204" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="212"/>
+      <c r="C58" s="205"/>
     </row>
     <row r="59" spans="2:3" ht="18.75">
       <c r="B59" s="118" t="s">
@@ -7174,10 +7152,10 @@
       </c>
     </row>
     <row r="66" spans="2:3" ht="26.25">
-      <c r="B66" s="200" t="s">
+      <c r="B66" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="201"/>
+      <c r="C66" s="219"/>
     </row>
     <row r="67" spans="2:3" ht="18.75">
       <c r="B67" s="115" t="s">
@@ -7224,10 +7202,10 @@
       <c r="C72" s="117"/>
     </row>
     <row r="73" spans="2:3" ht="26.25">
-      <c r="B73" s="200" t="s">
+      <c r="B73" s="218" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="201"/>
+      <c r="C73" s="219"/>
     </row>
     <row r="74" spans="2:3" ht="18.75">
       <c r="B74" s="119" t="s">
@@ -7290,10 +7268,10 @@
       <c r="C81" s="114"/>
     </row>
     <row r="82" spans="2:3" ht="28.5">
-      <c r="B82" s="217" t="s">
+      <c r="B82" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="C82" s="217"/>
+      <c r="C82" s="210"/>
     </row>
     <row r="83" spans="2:3" ht="19.5" thickBot="1">
       <c r="B83" s="126" t="s">
@@ -7364,10 +7342,10 @@
       <c r="C91" s="114"/>
     </row>
     <row r="92" spans="2:3" ht="26.25">
-      <c r="B92" s="206" t="s">
+      <c r="B92" s="200" t="s">
         <v>37</v>
       </c>
-      <c r="C92" s="207"/>
+      <c r="C92" s="201"/>
     </row>
     <row r="93" spans="2:3" ht="18.75">
       <c r="B93" s="115" t="s">
@@ -7386,10 +7364,10 @@
       </c>
     </row>
     <row r="95" spans="2:3" ht="26.25">
-      <c r="B95" s="206" t="s">
+      <c r="B95" s="200" t="s">
         <v>146</v>
       </c>
-      <c r="C95" s="207"/>
+      <c r="C95" s="201"/>
     </row>
     <row r="96" spans="2:3" ht="18.75">
       <c r="B96" s="115" t="s">
@@ -7452,10 +7430,10 @@
       <c r="C103" s="102"/>
     </row>
     <row r="104" spans="2:3" ht="36">
-      <c r="B104" s="205" t="s">
+      <c r="B104" s="223" t="s">
         <v>166</v>
       </c>
-      <c r="C104" s="205"/>
+      <c r="C104" s="223"/>
     </row>
     <row r="105" spans="2:3" ht="23.25">
       <c r="B105" s="36" t="s">
@@ -7490,10 +7468,10 @@
       </c>
     </row>
     <row r="110" spans="2:3" ht="26.25">
-      <c r="B110" s="204" t="s">
+      <c r="B110" s="222" t="s">
         <v>277</v>
       </c>
-      <c r="C110" s="204"/>
+      <c r="C110" s="222"/>
     </row>
     <row r="111" spans="2:3" ht="23.25">
       <c r="B111" s="47" t="s">
@@ -7528,10 +7506,10 @@
       </c>
     </row>
     <row r="116" spans="2:3" ht="31.5">
-      <c r="B116" s="202" t="s">
+      <c r="B116" s="220" t="s">
         <v>427</v>
       </c>
-      <c r="C116" s="203"/>
+      <c r="C116" s="221"/>
     </row>
     <row r="117" spans="2:3" ht="21">
       <c r="B117" s="149" t="s">
@@ -7583,6 +7561,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H12:J12"/>
@@ -7599,13 +7584,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B73:C73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B75" r:id="rId1" display="https://b2b.pramahikvision.com/goods/detail.html?goodsId=20829&amp;defaultViewProduct.productSapId=301313364&amp;selectType=all"/>
@@ -7637,22 +7615,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="174" t="s">
         <v>432</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
     </row>
     <row r="2" spans="1:20" ht="75" customHeight="1">
-      <c r="A2" s="176"/>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
+      <c r="A2" s="175"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
     </row>
     <row r="3" spans="1:20" ht="32.25" thickBot="1">
       <c r="A3" s="90" t="s">
@@ -7683,10 +7661,10 @@
       <c r="C5" s="152">
         <v>4200</v>
       </c>
-      <c r="F5" s="225">
+      <c r="F5" s="224">
         <v>76</v>
       </c>
-      <c r="H5" s="226">
+      <c r="H5" s="225">
         <v>76</v>
       </c>
     </row>
@@ -7700,8 +7678,8 @@
       <c r="C6" s="152">
         <v>4700</v>
       </c>
-      <c r="F6" s="225"/>
-      <c r="H6" s="226"/>
+      <c r="F6" s="224"/>
+      <c r="H6" s="225"/>
     </row>
     <row r="7" spans="1:20" ht="18">
       <c r="A7" s="150" t="s">
@@ -7713,8 +7691,8 @@
       <c r="C7" s="152">
         <v>5550</v>
       </c>
-      <c r="F7" s="225"/>
-      <c r="H7" s="226"/>
+      <c r="F7" s="224"/>
+      <c r="H7" s="225"/>
     </row>
     <row r="8" spans="1:20" ht="18">
       <c r="A8" s="150" t="s">
@@ -7726,8 +7704,8 @@
       <c r="C8" s="153">
         <v>5700</v>
       </c>
-      <c r="F8" s="225"/>
-      <c r="H8" s="226"/>
+      <c r="F8" s="224"/>
+      <c r="H8" s="225"/>
     </row>
     <row r="9" spans="1:20" ht="18">
       <c r="A9" s="150" t="s">
@@ -7739,8 +7717,8 @@
       <c r="C9" s="153">
         <v>6750</v>
       </c>
-      <c r="F9" s="225"/>
-      <c r="H9" s="226"/>
+      <c r="F9" s="224"/>
+      <c r="H9" s="225"/>
     </row>
     <row r="10" spans="1:20" ht="18">
       <c r="A10" s="87" t="s">
@@ -7750,8 +7728,8 @@
       <c r="C10" s="89">
         <v>11900</v>
       </c>
-      <c r="F10" s="225"/>
-      <c r="H10" s="226"/>
+      <c r="F10" s="224"/>
+      <c r="H10" s="225"/>
     </row>
     <row r="11" spans="1:20" ht="18">
       <c r="A11" s="150" t="s">
@@ -7763,8 +7741,8 @@
       <c r="C11" s="153">
         <v>6300</v>
       </c>
-      <c r="F11" s="225"/>
-      <c r="H11" s="226"/>
+      <c r="F11" s="224"/>
+      <c r="H11" s="225"/>
     </row>
     <row r="12" spans="1:20" ht="18">
       <c r="A12" s="150" t="s">
@@ -7776,8 +7754,8 @@
       <c r="C12" s="153">
         <v>9350</v>
       </c>
-      <c r="F12" s="225"/>
-      <c r="H12" s="226"/>
+      <c r="F12" s="224"/>
+      <c r="H12" s="225"/>
     </row>
     <row r="13" spans="1:20" ht="18">
       <c r="A13" s="150" t="s">
@@ -7801,10 +7779,10 @@
         <v>14500</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="170" t="s">
+      <c r="S14" s="169" t="s">
         <v>180</v>
       </c>
-      <c r="T14" s="170"/>
+      <c r="T14" s="169"/>
     </row>
     <row r="15" spans="1:20" ht="18">
       <c r="A15" s="150" t="s">
@@ -7935,10 +7913,10 @@
       <c r="C27" s="156">
         <v>5250</v>
       </c>
-      <c r="F27" s="226">
+      <c r="F27" s="225">
         <v>76</v>
       </c>
-      <c r="H27" s="226">
+      <c r="H27" s="225">
         <v>76</v>
       </c>
     </row>
@@ -7950,8 +7928,8 @@
       <c r="C28" s="156">
         <v>7200</v>
       </c>
-      <c r="F28" s="226"/>
-      <c r="H28" s="226"/>
+      <c r="F28" s="225"/>
+      <c r="H28" s="225"/>
     </row>
     <row r="29" spans="1:20" ht="18">
       <c r="A29" s="157" t="s">
@@ -7961,8 +7939,8 @@
       <c r="C29" s="156">
         <v>8750</v>
       </c>
-      <c r="F29" s="226"/>
-      <c r="H29" s="226"/>
+      <c r="F29" s="225"/>
+      <c r="H29" s="225"/>
     </row>
     <row r="30" spans="1:20" ht="18">
       <c r="A30" s="157" t="s">
@@ -7972,8 +7950,8 @@
       <c r="C30" s="156">
         <v>7400</v>
       </c>
-      <c r="F30" s="226"/>
-      <c r="H30" s="226"/>
+      <c r="F30" s="225"/>
+      <c r="H30" s="225"/>
     </row>
     <row r="31" spans="1:20" ht="18">
       <c r="A31" s="157" t="s">
@@ -7983,8 +7961,8 @@
       <c r="C31" s="156">
         <v>11300</v>
       </c>
-      <c r="F31" s="226"/>
-      <c r="H31" s="226"/>
+      <c r="F31" s="225"/>
+      <c r="H31" s="225"/>
     </row>
     <row r="32" spans="1:20" ht="18">
       <c r="A32" s="157" t="s">
@@ -7994,8 +7972,8 @@
       <c r="C32" s="156">
         <v>16900</v>
       </c>
-      <c r="F32" s="226"/>
-      <c r="H32" s="226"/>
+      <c r="F32" s="225"/>
+      <c r="H32" s="225"/>
     </row>
     <row r="33" spans="1:6" ht="18">
       <c r="A33" s="157" t="s">
@@ -8239,11 +8217,11 @@
       </c>
     </row>
     <row r="18" spans="4:6" ht="21">
-      <c r="D18" s="227" t="s">
+      <c r="D18" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="227"/>
-      <c r="F18" s="227"/>
+      <c r="E18" s="226"/>
+      <c r="F18" s="226"/>
     </row>
     <row r="19" spans="4:6" ht="21">
       <c r="D19" s="21" t="s">
@@ -8282,11 +8260,11 @@
       </c>
     </row>
     <row r="23" spans="4:6" ht="21">
-      <c r="D23" s="228" t="s">
+      <c r="D23" s="227" t="s">
         <v>164</v>
       </c>
-      <c r="E23" s="229"/>
-      <c r="F23" s="230"/>
+      <c r="E23" s="228"/>
+      <c r="F23" s="229"/>
     </row>
     <row r="24" spans="4:6" ht="21">
       <c r="D24" s="21" t="s">
@@ -8428,30 +8406,30 @@
   <sheetData>
     <row r="1" spans="6:12" hidden="1"/>
     <row r="2" spans="6:12">
-      <c r="G2" s="231" t="s">
+      <c r="G2" s="230" t="s">
         <v>432</v>
       </c>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
+      <c r="H2" s="231"/>
+      <c r="I2" s="231"/>
+      <c r="J2" s="231"/>
+      <c r="K2" s="231"/>
+      <c r="L2" s="231"/>
     </row>
     <row r="3" spans="6:12" ht="52.5" customHeight="1">
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
+      <c r="G3" s="231"/>
+      <c r="H3" s="231"/>
+      <c r="I3" s="231"/>
+      <c r="J3" s="231"/>
+      <c r="K3" s="231"/>
+      <c r="L3" s="231"/>
     </row>
     <row r="5" spans="6:12" ht="18">
-      <c r="F5" s="234" t="s">
+      <c r="F5" s="233" t="s">
         <v>197</v>
       </c>
-      <c r="G5" s="235"/>
-      <c r="H5" s="235"/>
-      <c r="I5" s="235"/>
+      <c r="G5" s="234"/>
+      <c r="H5" s="234"/>
+      <c r="I5" s="234"/>
     </row>
     <row r="6" spans="6:12" ht="63">
       <c r="F6" s="48" t="s">
@@ -8474,13 +8452,13 @@
       <c r="F7" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="236" t="s">
+      <c r="G7" s="235" t="s">
         <v>142</v>
       </c>
       <c r="H7" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="I7" s="237" t="s">
+      <c r="I7" s="236" t="s">
         <v>202</v>
       </c>
       <c r="J7" s="54">
@@ -8491,11 +8469,11 @@
       <c r="F8" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="G8" s="236"/>
+      <c r="G8" s="235"/>
       <c r="H8" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="I8" s="237"/>
+      <c r="I8" s="236"/>
       <c r="J8" s="54">
         <v>1993.95</v>
       </c>
@@ -8598,7 +8576,7 @@
       <c r="H15" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="I15" s="238" t="s">
+      <c r="I15" s="237" t="s">
         <v>296</v>
       </c>
       <c r="J15" s="68">
@@ -8613,7 +8591,7 @@
       <c r="H16" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="I16" s="239"/>
+      <c r="I16" s="238"/>
       <c r="J16" s="68">
         <v>3849.3</v>
       </c>
@@ -8622,11 +8600,11 @@
       <c r="F17" s="69" t="s">
         <v>217</v>
       </c>
-      <c r="G17" s="240"/>
+      <c r="G17" s="239"/>
       <c r="H17" s="70" t="s">
         <v>218</v>
       </c>
-      <c r="I17" s="233" t="s">
+      <c r="I17" s="232" t="s">
         <v>219</v>
       </c>
       <c r="J17" s="71">
@@ -8637,11 +8615,11 @@
       <c r="F18" s="69" t="s">
         <v>220</v>
       </c>
-      <c r="G18" s="240"/>
+      <c r="G18" s="239"/>
       <c r="H18" s="70" t="s">
         <v>221</v>
       </c>
-      <c r="I18" s="233"/>
+      <c r="I18" s="232"/>
       <c r="J18" s="71">
         <v>4141.2</v>
       </c>
@@ -8727,11 +8705,11 @@
       </c>
     </row>
     <row r="4" spans="4:6" ht="26.25">
-      <c r="D4" s="242" t="s">
+      <c r="D4" s="241" t="s">
         <v>333</v>
       </c>
-      <c r="E4" s="242"/>
-      <c r="F4" s="242"/>
+      <c r="E4" s="241"/>
+      <c r="F4" s="241"/>
     </row>
     <row r="5" spans="4:6" ht="23.25">
       <c r="D5" s="16" t="s">
@@ -8816,11 +8794,11 @@
       <c r="F12" s="17"/>
     </row>
     <row r="18" spans="4:6" ht="31.5">
-      <c r="D18" s="241" t="s">
+      <c r="D18" s="240" t="s">
         <v>332</v>
       </c>
-      <c r="E18" s="241"/>
-      <c r="F18" s="241"/>
+      <c r="E18" s="240"/>
+      <c r="F18" s="240"/>
     </row>
     <row r="19" spans="4:6" ht="23.25">
       <c r="D19" s="16" t="s">
@@ -8880,7 +8858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -8897,7 +8875,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="242" t="s">
         <v>436</v>
       </c>
     </row>
@@ -8907,7 +8885,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
-      <c r="B6" s="169" t="s">
+      <c r="B6" s="242" t="s">
         <v>437</v>
       </c>
     </row>

</xml_diff>

<commit_message>
This is a commit in the feature1 branch
</commit_message>
<xml_diff>
--- a/HIKVISION JUNE 2021 PRICE LIST (MOP).xlsx
+++ b/HIKVISION JUNE 2021 PRICE LIST (MOP).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\easo mathew\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meljo scans\AWS related\DEvOps 1\DEVOPSGITTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="HD DVR" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="EZVIZ" sheetId="7" r:id="rId7"/>
     <sheet name="BIOMETRIC" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
+    <sheet name="Committed sheet" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="441">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1430,6 +1431,9 @@
   </si>
   <si>
     <t>CAMERA</t>
+  </si>
+  <si>
+    <t>This is a new commit</t>
   </si>
 </sst>
 </file>
@@ -2876,6 +2880,7 @@
     <xf numFmtId="0" fontId="92" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2924,6 +2929,30 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2942,39 +2971,33 @@
     <xf numFmtId="0" fontId="65" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3023,24 +3046,6 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3095,7 +3100,6 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3135,7 +3139,7 @@
         <xdr:cNvPr id="2757" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F794545B-F0AD-4D5E-A9B7-5F7DD3D743EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F794545B-F0AD-4D5E-A9B7-5F7DD3D743EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3209,7 +3213,7 @@
         <xdr:cNvPr id="2758" name="图片 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D3C60F-939C-4EB5-9518-224E25F16960}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15D3C60F-939C-4EB5-9518-224E25F16960}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3288,7 +3292,7 @@
         <xdr:cNvPr id="14564" name="Picture 10" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F450D326-A10A-4C17-932A-29E325E7772B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F450D326-A10A-4C17-932A-29E325E7772B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3362,7 +3366,7 @@
         <xdr:cNvPr id="14565" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B7163B-A39D-4579-BF37-31F72DF3A3E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B7163B-A39D-4579-BF37-31F72DF3A3E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3436,7 +3440,7 @@
         <xdr:cNvPr id="14566" name="Picture 12" descr="Image result for CS-X5C-4APEC">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEF73321-D25C-4263-A062-A8A4A50B64A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEF73321-D25C-4263-A062-A8A4A50B64A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3510,7 +3514,7 @@
         <xdr:cNvPr id="14567" name="Picture 13" descr="Image result for C1C CAMERA">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FABD93E-A38C-433B-ACE6-ABABF15DE2DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4FABD93E-A38C-433B-ACE6-ABABF15DE2DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3584,7 +3588,7 @@
         <xdr:cNvPr id="14568" name="Picture 14" descr="Image result for CS-CV346-AO-7A3WFR(3MP)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77CFCDF6-B04D-4EC4-AC5D-ED82A54AB919}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{77CFCDF6-B04D-4EC4-AC5D-ED82A54AB919}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3658,7 +3662,7 @@
         <xdr:cNvPr id="14569" name="Picture 15" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F14B0F-DD82-40C8-B42B-F711EB4B66F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A2F14B0F-DD82-40C8-B42B-F711EB4B66F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3732,7 +3736,7 @@
         <xdr:cNvPr id="14570" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45B85A1-918B-48CB-9D61-7AB33CABEF38}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A45B85A1-918B-48CB-9D61-7AB33CABEF38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3806,7 +3810,7 @@
         <xdr:cNvPr id="14571" name="Picture 15" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6B0AD6D-C36D-4E0A-81DD-DF43FC954379}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6B0AD6D-C36D-4E0A-81DD-DF43FC954379}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3880,7 +3884,7 @@
         <xdr:cNvPr id="14572" name="Picture 11" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2C1C4E-39B8-419D-8C58-48DCE0C63BA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB2C1C4E-39B8-419D-8C58-48DCE0C63BA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3954,7 +3958,7 @@
         <xdr:cNvPr id="14573" name="AutoShape 3" descr="Image result for CS-CV310-A0-1B2WFR">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58FE2307-73C2-4B94-A8A4-6F0CE4F0ACFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{58FE2307-73C2-4B94-A8A4-6F0CE4F0ACFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4015,7 +4019,7 @@
         <xdr:cNvPr id="14574" name="Picture 13" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7080737-A6C9-4FBB-B8A4-29BA5D8D30DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B7080737-A6C9-4FBB-B8A4-29BA5D8D30DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4089,7 +4093,7 @@
         <xdr:cNvPr id="14575" name="Picture 15" descr="Image result for C1C CAMERA">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0B5B8F1-63F4-4958-B1D3-30B9BA7F7815}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E0B5B8F1-63F4-4958-B1D3-30B9BA7F7815}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4163,7 +4167,7 @@
         <xdr:cNvPr id="14576" name="Picture 16" descr="Image result for CS-CV346-AO-7A3WFR(3MP)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2ED700-160A-4191-A9B9-F382F2F9E451}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CF2ED700-160A-4191-A9B9-F382F2F9E451}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4237,7 +4241,7 @@
         <xdr:cNvPr id="14577" name="Picture 17" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBFB5773-8A75-4665-AC47-44CC01BB972B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBFB5773-8A75-4665-AC47-44CC01BB972B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4311,7 +4315,7 @@
         <xdr:cNvPr id="14578" name="Picture 18" descr="Related image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E035C21-C91C-4651-B4FD-A1ECA30E860D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E035C21-C91C-4651-B4FD-A1ECA30E860D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4385,7 +4389,7 @@
         <xdr:cNvPr id="14579" name="Picture 19" descr="Image result for EZVIZ NVR KIT">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397FF8EE-BFB2-4FE7-A3B2-F9942321552C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{397FF8EE-BFB2-4FE7-A3B2-F9942321552C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4459,7 +4463,7 @@
         <xdr:cNvPr id="14580" name="Picture 20" descr="Camera IP EZVIZ CS-C3N (A0-3H2WFRL) 1080P Có Màu Ban Đêm - Hàng ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B46A902-DED4-4EA9-A473-659B44C1B7AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8B46A902-DED4-4EA9-A473-659B44C1B7AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4533,7 +4537,7 @@
         <xdr:cNvPr id="14581" name="Picture 21" descr="Camera IP EZVIZ CS-C3N (A0-3H2WFRL) 1080P Có Màu Ban Đêm - Hàng ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691C9B81-B5BB-4F80-A630-EAF4F98C6EB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{691C9B81-B5BB-4F80-A630-EAF4F98C6EB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4607,7 +4611,7 @@
         <xdr:cNvPr id="14582" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7354854F-34EB-4903-A01B-7844B435C044}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7354854F-34EB-4903-A01B-7844B435C044}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4973,22 +4977,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="2:17" ht="86.25" customHeight="1">
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="32" t="s">
@@ -5000,10 +5004,10 @@
       <c r="F3" s="41"/>
     </row>
     <row r="4" spans="2:17" ht="23.25">
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="180" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="180"/>
+      <c r="C4" s="181"/>
     </row>
     <row r="5" spans="2:17" ht="15.75">
       <c r="B5" s="128" t="s">
@@ -5012,7 +5016,7 @@
       <c r="C5" s="84">
         <v>2900</v>
       </c>
-      <c r="G5" s="177"/>
+      <c r="G5" s="178"/>
     </row>
     <row r="6" spans="2:17" ht="15.75">
       <c r="B6" s="128" t="s">
@@ -5021,11 +5025,11 @@
       <c r="C6" s="84">
         <v>4340</v>
       </c>
-      <c r="G6" s="177"/>
-      <c r="P6" s="169" t="s">
+      <c r="G6" s="178"/>
+      <c r="P6" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="Q6" s="169"/>
+      <c r="Q6" s="170"/>
     </row>
     <row r="7" spans="2:17" ht="15.75">
       <c r="B7" s="128" t="s">
@@ -5034,7 +5038,7 @@
       <c r="C7" s="84">
         <v>7550</v>
       </c>
-      <c r="G7" s="177"/>
+      <c r="G7" s="178"/>
       <c r="O7" s="11" t="s">
         <v>39</v>
       </c>
@@ -5046,10 +5050,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" ht="23.25">
-      <c r="B8" s="181" t="s">
+      <c r="B8" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="182"/>
+      <c r="C8" s="183"/>
       <c r="G8" s="25"/>
       <c r="O8" s="11"/>
       <c r="P8" s="42"/>
@@ -5062,7 +5066,7 @@
       <c r="C9" s="130">
         <v>2350</v>
       </c>
-      <c r="G9" s="178" t="s">
+      <c r="G9" s="179" t="s">
         <v>66</v>
       </c>
       <c r="O9" s="11"/>
@@ -5076,7 +5080,7 @@
       <c r="C10" s="130">
         <v>3550</v>
       </c>
-      <c r="G10" s="178"/>
+      <c r="G10" s="179"/>
       <c r="O10" s="11"/>
       <c r="P10" s="42"/>
       <c r="Q10" s="11"/>
@@ -5088,7 +5092,7 @@
       <c r="C11" s="130">
         <v>5950</v>
       </c>
-      <c r="G11" s="178"/>
+      <c r="G11" s="179"/>
       <c r="O11" s="11"/>
       <c r="P11" s="42"/>
       <c r="Q11" s="11"/>
@@ -5100,7 +5104,7 @@
       <c r="C12" s="130">
         <v>5950</v>
       </c>
-      <c r="G12" s="178"/>
+      <c r="G12" s="179"/>
       <c r="O12" s="11"/>
       <c r="P12" s="42"/>
       <c r="Q12" s="11"/>
@@ -5112,7 +5116,7 @@
       <c r="C13" s="130">
         <v>8200</v>
       </c>
-      <c r="G13" s="178"/>
+      <c r="G13" s="179"/>
       <c r="O13" s="11"/>
       <c r="P13" s="42"/>
       <c r="Q13" s="11"/>
@@ -5124,17 +5128,17 @@
       <c r="C14" s="130">
         <v>17500</v>
       </c>
-      <c r="G14" s="178"/>
+      <c r="G14" s="179"/>
       <c r="O14" s="43"/>
       <c r="P14" s="44"/>
       <c r="Q14" s="43"/>
     </row>
     <row r="15" spans="2:17" ht="23.25">
-      <c r="B15" s="181" t="s">
+      <c r="B15" s="182" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="182"/>
-      <c r="G15" s="178"/>
+      <c r="C15" s="183"/>
+      <c r="G15" s="179"/>
       <c r="P15" s="41"/>
     </row>
     <row r="16" spans="2:17" ht="15.75">
@@ -5144,7 +5148,7 @@
       <c r="C16" s="130">
         <v>10500</v>
       </c>
-      <c r="G16" s="178"/>
+      <c r="G16" s="179"/>
       <c r="P16" s="41"/>
     </row>
     <row r="17" spans="2:16" ht="15.75">
@@ -5154,7 +5158,7 @@
       <c r="C17" s="130">
         <v>14500</v>
       </c>
-      <c r="G17" s="178"/>
+      <c r="G17" s="179"/>
       <c r="P17" s="41"/>
     </row>
     <row r="18" spans="2:16" ht="15.75">
@@ -5164,7 +5168,7 @@
       <c r="C18" s="130">
         <v>3900</v>
       </c>
-      <c r="G18" s="178"/>
+      <c r="G18" s="179"/>
       <c r="P18" s="41"/>
     </row>
     <row r="19" spans="2:16" ht="15.75">
@@ -5174,7 +5178,7 @@
       <c r="C19" s="130">
         <v>5720</v>
       </c>
-      <c r="G19" s="178"/>
+      <c r="G19" s="179"/>
       <c r="P19" s="41"/>
     </row>
     <row r="20" spans="2:16" ht="15.75">
@@ -5184,7 +5188,7 @@
       <c r="C20" s="130">
         <v>9800</v>
       </c>
-      <c r="G20" s="178"/>
+      <c r="G20" s="179"/>
       <c r="P20" s="41"/>
     </row>
     <row r="21" spans="2:16" ht="15.75">
@@ -5194,7 +5198,7 @@
       <c r="C21" s="130">
         <v>7900</v>
       </c>
-      <c r="G21" s="178"/>
+      <c r="G21" s="179"/>
       <c r="P21" s="41"/>
     </row>
     <row r="22" spans="2:16" ht="15.75">
@@ -5204,15 +5208,15 @@
       <c r="C22" s="130">
         <v>11500</v>
       </c>
-      <c r="G22" s="178"/>
+      <c r="G22" s="179"/>
       <c r="P22" s="41"/>
     </row>
     <row r="23" spans="2:16" ht="20.25">
-      <c r="B23" s="183" t="s">
+      <c r="B23" s="184" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="184"/>
-      <c r="G23" s="178"/>
+      <c r="C23" s="185"/>
+      <c r="G23" s="179"/>
       <c r="P23" s="41"/>
     </row>
     <row r="24" spans="2:16" ht="15.75">
@@ -5222,7 +5226,7 @@
       <c r="C24" s="84" t="s">
         <v>384</v>
       </c>
-      <c r="G24" s="178"/>
+      <c r="G24" s="179"/>
       <c r="P24" s="41"/>
     </row>
     <row r="25" spans="2:16" ht="15.75">
@@ -5232,7 +5236,7 @@
       <c r="C25" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="G25" s="178"/>
+      <c r="G25" s="179"/>
       <c r="P25" s="41"/>
     </row>
     <row r="26" spans="2:16" ht="15.75">
@@ -5242,7 +5246,7 @@
       <c r="C26" s="84">
         <v>0</v>
       </c>
-      <c r="G26" s="178"/>
+      <c r="G26" s="179"/>
       <c r="P26" s="41"/>
     </row>
     <row r="27" spans="2:16" ht="15.75">
@@ -5252,7 +5256,7 @@
       <c r="C27" s="84" t="s">
         <v>386</v>
       </c>
-      <c r="G27" s="178"/>
+      <c r="G27" s="179"/>
       <c r="P27" s="41"/>
     </row>
     <row r="28" spans="2:16" ht="15.75">
@@ -5262,7 +5266,7 @@
       <c r="C28" s="84">
         <v>17000</v>
       </c>
-      <c r="G28" s="178"/>
+      <c r="G28" s="179"/>
     </row>
     <row r="29" spans="2:16" ht="15.75">
       <c r="B29" s="128" t="s">
@@ -5274,10 +5278,10 @@
       <c r="G29" s="40"/>
     </row>
     <row r="30" spans="2:16" ht="26.25">
-      <c r="B30" s="172" t="s">
+      <c r="B30" s="173" t="s">
         <v>276</v>
       </c>
-      <c r="C30" s="173"/>
+      <c r="C30" s="174"/>
     </row>
     <row r="31" spans="2:16" ht="15.75">
       <c r="B31" s="131" t="s">
@@ -5296,10 +5300,10 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="20.25">
-      <c r="B35" s="176" t="s">
+      <c r="B35" s="177" t="s">
         <v>152</v>
       </c>
-      <c r="C35" s="176"/>
+      <c r="C35" s="177"/>
     </row>
     <row r="36" spans="2:4" ht="15.75">
       <c r="B36" s="86" t="s">
@@ -5330,10 +5334,10 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="20.25">
-      <c r="B40" s="170" t="s">
+      <c r="B40" s="171" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="170"/>
+      <c r="C40" s="171"/>
     </row>
     <row r="41" spans="2:4" ht="15.75">
       <c r="B41" s="131" t="s">
@@ -5358,10 +5362,10 @@
       <c r="C43" s="132"/>
     </row>
     <row r="45" spans="2:4" ht="18">
-      <c r="B45" s="171" t="s">
+      <c r="B45" s="172" t="s">
         <v>154</v>
       </c>
-      <c r="C45" s="171"/>
+      <c r="C45" s="172"/>
     </row>
     <row r="46" spans="2:4" ht="15.75">
       <c r="B46" s="131" t="s">
@@ -5412,6 +5416,26 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5437,39 +5461,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="2:10" ht="87.75" customHeight="1">
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="2:10" ht="15.75">
       <c r="B3" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="35"/>
-      <c r="H3" s="191" t="s">
+      <c r="H3" s="186" t="s">
         <v>431</v>
       </c>
-      <c r="I3" s="191"/>
-      <c r="J3" s="191"/>
+      <c r="I3" s="186"/>
+      <c r="J3" s="186"/>
     </row>
     <row r="4" spans="2:10" ht="26.25">
-      <c r="B4" s="194" t="s">
+      <c r="B4" s="189" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="195"/>
+      <c r="C4" s="190"/>
       <c r="H4" s="45" t="s">
         <v>337</v>
       </c>
@@ -5537,11 +5561,11 @@
       <c r="C9" s="130">
         <v>1600</v>
       </c>
-      <c r="H9" s="192" t="s">
+      <c r="H9" s="187" t="s">
         <v>341</v>
       </c>
-      <c r="I9" s="192"/>
-      <c r="J9" s="192"/>
+      <c r="I9" s="187"/>
+      <c r="J9" s="187"/>
     </row>
     <row r="10" spans="2:10" ht="30">
       <c r="B10" s="141" t="s">
@@ -5619,10 +5643,10 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="27">
-      <c r="B16" s="196" t="s">
+      <c r="B16" s="191" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="197"/>
+      <c r="C16" s="192"/>
     </row>
     <row r="17" spans="2:3" ht="17.25">
       <c r="B17" s="142" t="s">
@@ -5773,10 +5797,10 @@
       <c r="C35" s="12"/>
     </row>
     <row r="36" spans="2:3" ht="20.25">
-      <c r="B36" s="198" t="s">
+      <c r="B36" s="193" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="198"/>
+      <c r="C36" s="193"/>
     </row>
     <row r="37" spans="2:3" ht="15.75">
       <c r="B37" s="146" t="s">
@@ -5875,10 +5899,10 @@
       <c r="C49" s="1"/>
     </row>
     <row r="51" spans="2:16" ht="23.25">
-      <c r="B51" s="193" t="s">
+      <c r="B51" s="188" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="193"/>
+      <c r="C51" s="188"/>
     </row>
     <row r="52" spans="2:16" ht="17.25">
       <c r="B52" s="141" t="s">
@@ -5927,10 +5951,10 @@
       <c r="C57" s="140">
         <v>870</v>
       </c>
-      <c r="O57" s="169" t="s">
+      <c r="O57" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="P57" s="169"/>
+      <c r="P57" s="170"/>
     </row>
     <row r="58" spans="2:16">
       <c r="B58" s="28"/>
@@ -5946,10 +5970,10 @@
       </c>
     </row>
     <row r="59" spans="2:16" ht="23.25">
-      <c r="B59" s="187" t="s">
+      <c r="B59" s="196" t="s">
         <v>160</v>
       </c>
-      <c r="C59" s="187"/>
+      <c r="C59" s="196"/>
       <c r="N59" s="11"/>
       <c r="O59" s="42"/>
       <c r="P59" s="11"/>
@@ -6044,10 +6068,10 @@
       <c r="C69" s="12"/>
     </row>
     <row r="70" spans="2:3" ht="23.25">
-      <c r="B70" s="187" t="s">
+      <c r="B70" s="196" t="s">
         <v>161</v>
       </c>
-      <c r="C70" s="187"/>
+      <c r="C70" s="196"/>
     </row>
     <row r="71" spans="2:3">
       <c r="B71" s="13" t="s">
@@ -6070,10 +6094,10 @@
       <c r="C73" s="27"/>
     </row>
     <row r="74" spans="2:3" ht="23.25">
-      <c r="B74" s="188" t="s">
+      <c r="B74" s="197" t="s">
         <v>162</v>
       </c>
-      <c r="C74" s="188"/>
+      <c r="C74" s="197"/>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="13" t="s">
@@ -6136,10 +6160,10 @@
       <c r="C82" s="27"/>
     </row>
     <row r="83" spans="1:3" ht="18">
-      <c r="B83" s="189" t="s">
+      <c r="B83" s="198" t="s">
         <v>163</v>
       </c>
-      <c r="C83" s="189"/>
+      <c r="C83" s="198"/>
     </row>
     <row r="84" spans="1:3">
       <c r="B84" s="24" t="s">
@@ -6178,10 +6202,10 @@
       <c r="C88" s="31"/>
     </row>
     <row r="89" spans="1:3" ht="23.25">
-      <c r="B89" s="190" t="s">
+      <c r="B89" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="C89" s="190"/>
+      <c r="C89" s="199"/>
     </row>
     <row r="90" spans="1:3" ht="18.75">
       <c r="A90" s="139"/>
@@ -6256,14 +6280,14 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="B99" s="186" t="s">
+      <c r="B99" s="195" t="s">
         <v>272</v>
       </c>
-      <c r="C99" s="186"/>
+      <c r="C99" s="195"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="B100" s="186"/>
-      <c r="C100" s="186"/>
+      <c r="B100" s="195"/>
+      <c r="C100" s="195"/>
     </row>
     <row r="101" spans="1:3">
       <c r="B101" s="45" t="s">
@@ -6282,10 +6306,10 @@
       </c>
     </row>
     <row r="105" spans="1:3" ht="23.25">
-      <c r="B105" s="185" t="s">
+      <c r="B105" s="194" t="s">
         <v>285</v>
       </c>
-      <c r="C105" s="185"/>
+      <c r="C105" s="194"/>
     </row>
     <row r="106" spans="1:3" ht="18.75">
       <c r="B106" s="148" t="s">
@@ -6313,6 +6337,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B99:C100"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B89:C89"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="B1:G2"/>
@@ -6321,13 +6352,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B99:C100"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B89:C89"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B90" r:id="rId1" display="https://b2b.pramahikvision.com/goods/detail.html?goodsId=19672&amp;defaultViewProduct.productSapId=300611637&amp;selectType=all"/>
@@ -6370,22 +6394,22 @@
       <c r="E1" s="163"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
     </row>
     <row r="3" spans="1:6" ht="42" customHeight="1">
-      <c r="A3" s="175"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
+      <c r="A3" s="176"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="176"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="164"/>
@@ -6555,39 +6579,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
     </row>
     <row r="2" spans="2:10" ht="69" customHeight="1">
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
     </row>
     <row r="3" spans="2:10" ht="23.25">
-      <c r="B3" s="216" t="s">
+      <c r="B3" s="223" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="217"/>
-      <c r="H3" s="199" t="s">
+      <c r="C3" s="224"/>
+      <c r="H3" s="208" t="s">
         <v>346</v>
       </c>
-      <c r="I3" s="199"/>
-      <c r="J3" s="199"/>
+      <c r="I3" s="208"/>
+      <c r="J3" s="208"/>
     </row>
     <row r="4" spans="2:10" ht="23.25">
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="211" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="205"/>
+      <c r="C4" s="212"/>
       <c r="H4" s="45" t="s">
         <v>347</v>
       </c>
@@ -6627,10 +6651,10 @@
       <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:10" ht="26.25">
-      <c r="B7" s="206" t="s">
+      <c r="B7" s="213" t="s">
         <v>237</v>
       </c>
-      <c r="C7" s="206"/>
+      <c r="C7" s="213"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -6677,15 +6701,15 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="23.25">
-      <c r="B12" s="214" t="s">
+      <c r="B12" s="221" t="s">
         <v>254</v>
       </c>
-      <c r="C12" s="214"/>
-      <c r="H12" s="199" t="s">
+      <c r="C12" s="221"/>
+      <c r="H12" s="208" t="s">
         <v>357</v>
       </c>
-      <c r="I12" s="199"/>
-      <c r="J12" s="199"/>
+      <c r="I12" s="208"/>
+      <c r="J12" s="208"/>
     </row>
     <row r="13" spans="2:10" ht="18">
       <c r="B13" s="108" t="s">
@@ -6733,10 +6757,10 @@
       <c r="J15" s="17"/>
     </row>
     <row r="16" spans="2:10" ht="23.25">
-      <c r="B16" s="211" t="s">
+      <c r="B16" s="218" t="s">
         <v>255</v>
       </c>
-      <c r="C16" s="211"/>
+      <c r="C16" s="218"/>
       <c r="H16" s="45" t="s">
         <v>353</v>
       </c>
@@ -6776,15 +6800,15 @@
       <c r="C20" s="113"/>
     </row>
     <row r="21" spans="2:16" ht="23.25">
-      <c r="B21" s="215" t="s">
+      <c r="B21" s="222" t="s">
         <v>238</v>
       </c>
-      <c r="C21" s="215"/>
+      <c r="C21" s="222"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="169" t="s">
+      <c r="O21" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="P21" s="169"/>
+      <c r="P21" s="170"/>
     </row>
     <row r="22" spans="2:16" ht="18">
       <c r="B22" s="105" t="s">
@@ -6848,10 +6872,10 @@
       <c r="P26" s="11"/>
     </row>
     <row r="27" spans="2:16" ht="23.25">
-      <c r="B27" s="207" t="s">
+      <c r="B27" s="214" t="s">
         <v>241</v>
       </c>
-      <c r="C27" s="207"/>
+      <c r="C27" s="214"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
@@ -6924,10 +6948,10 @@
       <c r="C34" s="104"/>
     </row>
     <row r="35" spans="2:3" ht="23.25">
-      <c r="B35" s="212" t="s">
+      <c r="B35" s="219" t="s">
         <v>334</v>
       </c>
-      <c r="C35" s="213"/>
+      <c r="C35" s="220"/>
     </row>
     <row r="36" spans="2:3" ht="18">
       <c r="B36" s="107" t="s">
@@ -6946,10 +6970,10 @@
       </c>
     </row>
     <row r="38" spans="2:3" ht="23.25">
-      <c r="B38" s="208" t="s">
+      <c r="B38" s="215" t="s">
         <v>242</v>
       </c>
-      <c r="C38" s="209"/>
+      <c r="C38" s="216"/>
     </row>
     <row r="39" spans="2:3" ht="18.75">
       <c r="B39" s="115" t="s">
@@ -6968,10 +6992,10 @@
       </c>
     </row>
     <row r="41" spans="2:3" ht="18">
-      <c r="B41" s="202" t="s">
+      <c r="B41" s="209" t="s">
         <v>243</v>
       </c>
-      <c r="C41" s="203"/>
+      <c r="C41" s="210"/>
     </row>
     <row r="42" spans="2:3" ht="18">
       <c r="B42" s="107" t="s">
@@ -7094,10 +7118,10 @@
       <c r="C57" s="102"/>
     </row>
     <row r="58" spans="2:3" ht="23.25">
-      <c r="B58" s="204" t="s">
+      <c r="B58" s="211" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="205"/>
+      <c r="C58" s="212"/>
     </row>
     <row r="59" spans="2:3" ht="18.75">
       <c r="B59" s="118" t="s">
@@ -7152,10 +7176,10 @@
       </c>
     </row>
     <row r="66" spans="2:3" ht="26.25">
-      <c r="B66" s="218" t="s">
+      <c r="B66" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="219"/>
+      <c r="C66" s="201"/>
     </row>
     <row r="67" spans="2:3" ht="18.75">
       <c r="B67" s="115" t="s">
@@ -7202,10 +7226,10 @@
       <c r="C72" s="117"/>
     </row>
     <row r="73" spans="2:3" ht="26.25">
-      <c r="B73" s="218" t="s">
+      <c r="B73" s="200" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="219"/>
+      <c r="C73" s="201"/>
     </row>
     <row r="74" spans="2:3" ht="18.75">
       <c r="B74" s="119" t="s">
@@ -7268,10 +7292,10 @@
       <c r="C81" s="114"/>
     </row>
     <row r="82" spans="2:3" ht="28.5">
-      <c r="B82" s="210" t="s">
+      <c r="B82" s="217" t="s">
         <v>36</v>
       </c>
-      <c r="C82" s="210"/>
+      <c r="C82" s="217"/>
     </row>
     <row r="83" spans="2:3" ht="19.5" thickBot="1">
       <c r="B83" s="126" t="s">
@@ -7342,10 +7366,10 @@
       <c r="C91" s="114"/>
     </row>
     <row r="92" spans="2:3" ht="26.25">
-      <c r="B92" s="200" t="s">
+      <c r="B92" s="206" t="s">
         <v>37</v>
       </c>
-      <c r="C92" s="201"/>
+      <c r="C92" s="207"/>
     </row>
     <row r="93" spans="2:3" ht="18.75">
       <c r="B93" s="115" t="s">
@@ -7364,10 +7388,10 @@
       </c>
     </row>
     <row r="95" spans="2:3" ht="26.25">
-      <c r="B95" s="200" t="s">
+      <c r="B95" s="206" t="s">
         <v>146</v>
       </c>
-      <c r="C95" s="201"/>
+      <c r="C95" s="207"/>
     </row>
     <row r="96" spans="2:3" ht="18.75">
       <c r="B96" s="115" t="s">
@@ -7430,10 +7454,10 @@
       <c r="C103" s="102"/>
     </row>
     <row r="104" spans="2:3" ht="36">
-      <c r="B104" s="223" t="s">
+      <c r="B104" s="205" t="s">
         <v>166</v>
       </c>
-      <c r="C104" s="223"/>
+      <c r="C104" s="205"/>
     </row>
     <row r="105" spans="2:3" ht="23.25">
       <c r="B105" s="36" t="s">
@@ -7468,10 +7492,10 @@
       </c>
     </row>
     <row r="110" spans="2:3" ht="26.25">
-      <c r="B110" s="222" t="s">
+      <c r="B110" s="204" t="s">
         <v>277</v>
       </c>
-      <c r="C110" s="222"/>
+      <c r="C110" s="204"/>
     </row>
     <row r="111" spans="2:3" ht="23.25">
       <c r="B111" s="47" t="s">
@@ -7506,10 +7530,10 @@
       </c>
     </row>
     <row r="116" spans="2:3" ht="31.5">
-      <c r="B116" s="220" t="s">
+      <c r="B116" s="202" t="s">
         <v>427</v>
       </c>
-      <c r="C116" s="221"/>
+      <c r="C116" s="203"/>
     </row>
     <row r="117" spans="2:3" ht="21">
       <c r="B117" s="149" t="s">
@@ -7561,13 +7585,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B73:C73"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H12:J12"/>
@@ -7584,6 +7601,13 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B73:C73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B75" r:id="rId1" display="https://b2b.pramahikvision.com/goods/detail.html?goodsId=20829&amp;defaultViewProduct.productSapId=301313364&amp;selectType=all"/>
@@ -7615,22 +7639,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="175" t="s">
         <v>432</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
     </row>
     <row r="2" spans="1:20" ht="75" customHeight="1">
-      <c r="A2" s="175"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="A2" s="176"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
     </row>
     <row r="3" spans="1:20" ht="32.25" thickBot="1">
       <c r="A3" s="90" t="s">
@@ -7661,10 +7685,10 @@
       <c r="C5" s="152">
         <v>4200</v>
       </c>
-      <c r="F5" s="224">
+      <c r="F5" s="225">
         <v>76</v>
       </c>
-      <c r="H5" s="225">
+      <c r="H5" s="226">
         <v>76</v>
       </c>
     </row>
@@ -7678,8 +7702,8 @@
       <c r="C6" s="152">
         <v>4700</v>
       </c>
-      <c r="F6" s="224"/>
-      <c r="H6" s="225"/>
+      <c r="F6" s="225"/>
+      <c r="H6" s="226"/>
     </row>
     <row r="7" spans="1:20" ht="18">
       <c r="A7" s="150" t="s">
@@ -7691,8 +7715,8 @@
       <c r="C7" s="152">
         <v>5550</v>
       </c>
-      <c r="F7" s="224"/>
-      <c r="H7" s="225"/>
+      <c r="F7" s="225"/>
+      <c r="H7" s="226"/>
     </row>
     <row r="8" spans="1:20" ht="18">
       <c r="A8" s="150" t="s">
@@ -7704,8 +7728,8 @@
       <c r="C8" s="153">
         <v>5700</v>
       </c>
-      <c r="F8" s="224"/>
-      <c r="H8" s="225"/>
+      <c r="F8" s="225"/>
+      <c r="H8" s="226"/>
     </row>
     <row r="9" spans="1:20" ht="18">
       <c r="A9" s="150" t="s">
@@ -7717,8 +7741,8 @@
       <c r="C9" s="153">
         <v>6750</v>
       </c>
-      <c r="F9" s="224"/>
-      <c r="H9" s="225"/>
+      <c r="F9" s="225"/>
+      <c r="H9" s="226"/>
     </row>
     <row r="10" spans="1:20" ht="18">
       <c r="A10" s="87" t="s">
@@ -7728,8 +7752,8 @@
       <c r="C10" s="89">
         <v>11900</v>
       </c>
-      <c r="F10" s="224"/>
-      <c r="H10" s="225"/>
+      <c r="F10" s="225"/>
+      <c r="H10" s="226"/>
     </row>
     <row r="11" spans="1:20" ht="18">
       <c r="A11" s="150" t="s">
@@ -7741,8 +7765,8 @@
       <c r="C11" s="153">
         <v>6300</v>
       </c>
-      <c r="F11" s="224"/>
-      <c r="H11" s="225"/>
+      <c r="F11" s="225"/>
+      <c r="H11" s="226"/>
     </row>
     <row r="12" spans="1:20" ht="18">
       <c r="A12" s="150" t="s">
@@ -7754,8 +7778,8 @@
       <c r="C12" s="153">
         <v>9350</v>
       </c>
-      <c r="F12" s="224"/>
-      <c r="H12" s="225"/>
+      <c r="F12" s="225"/>
+      <c r="H12" s="226"/>
     </row>
     <row r="13" spans="1:20" ht="18">
       <c r="A13" s="150" t="s">
@@ -7779,10 +7803,10 @@
         <v>14500</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="169" t="s">
+      <c r="S14" s="170" t="s">
         <v>180</v>
       </c>
-      <c r="T14" s="169"/>
+      <c r="T14" s="170"/>
     </row>
     <row r="15" spans="1:20" ht="18">
       <c r="A15" s="150" t="s">
@@ -7913,10 +7937,10 @@
       <c r="C27" s="156">
         <v>5250</v>
       </c>
-      <c r="F27" s="225">
+      <c r="F27" s="226">
         <v>76</v>
       </c>
-      <c r="H27" s="225">
+      <c r="H27" s="226">
         <v>76</v>
       </c>
     </row>
@@ -7928,8 +7952,8 @@
       <c r="C28" s="156">
         <v>7200</v>
       </c>
-      <c r="F28" s="225"/>
-      <c r="H28" s="225"/>
+      <c r="F28" s="226"/>
+      <c r="H28" s="226"/>
     </row>
     <row r="29" spans="1:20" ht="18">
       <c r="A29" s="157" t="s">
@@ -7939,8 +7963,8 @@
       <c r="C29" s="156">
         <v>8750</v>
       </c>
-      <c r="F29" s="225"/>
-      <c r="H29" s="225"/>
+      <c r="F29" s="226"/>
+      <c r="H29" s="226"/>
     </row>
     <row r="30" spans="1:20" ht="18">
       <c r="A30" s="157" t="s">
@@ -7950,8 +7974,8 @@
       <c r="C30" s="156">
         <v>7400</v>
       </c>
-      <c r="F30" s="225"/>
-      <c r="H30" s="225"/>
+      <c r="F30" s="226"/>
+      <c r="H30" s="226"/>
     </row>
     <row r="31" spans="1:20" ht="18">
       <c r="A31" s="157" t="s">
@@ -7961,8 +7985,8 @@
       <c r="C31" s="156">
         <v>11300</v>
       </c>
-      <c r="F31" s="225"/>
-      <c r="H31" s="225"/>
+      <c r="F31" s="226"/>
+      <c r="H31" s="226"/>
     </row>
     <row r="32" spans="1:20" ht="18">
       <c r="A32" s="157" t="s">
@@ -7972,8 +7996,8 @@
       <c r="C32" s="156">
         <v>16900</v>
       </c>
-      <c r="F32" s="225"/>
-      <c r="H32" s="225"/>
+      <c r="F32" s="226"/>
+      <c r="H32" s="226"/>
     </row>
     <row r="33" spans="1:6" ht="18">
       <c r="A33" s="157" t="s">
@@ -8217,11 +8241,11 @@
       </c>
     </row>
     <row r="18" spans="4:6" ht="21">
-      <c r="D18" s="226" t="s">
+      <c r="D18" s="227" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="226"/>
-      <c r="F18" s="226"/>
+      <c r="E18" s="227"/>
+      <c r="F18" s="227"/>
     </row>
     <row r="19" spans="4:6" ht="21">
       <c r="D19" s="21" t="s">
@@ -8260,11 +8284,11 @@
       </c>
     </row>
     <row r="23" spans="4:6" ht="21">
-      <c r="D23" s="227" t="s">
+      <c r="D23" s="228" t="s">
         <v>164</v>
       </c>
-      <c r="E23" s="228"/>
-      <c r="F23" s="229"/>
+      <c r="E23" s="229"/>
+      <c r="F23" s="230"/>
     </row>
     <row r="24" spans="4:6" ht="21">
       <c r="D24" s="21" t="s">
@@ -8406,30 +8430,30 @@
   <sheetData>
     <row r="1" spans="6:12" hidden="1"/>
     <row r="2" spans="6:12">
-      <c r="G2" s="230" t="s">
+      <c r="G2" s="231" t="s">
         <v>432</v>
       </c>
-      <c r="H2" s="231"/>
-      <c r="I2" s="231"/>
-      <c r="J2" s="231"/>
-      <c r="K2" s="231"/>
-      <c r="L2" s="231"/>
+      <c r="H2" s="232"/>
+      <c r="I2" s="232"/>
+      <c r="J2" s="232"/>
+      <c r="K2" s="232"/>
+      <c r="L2" s="232"/>
     </row>
     <row r="3" spans="6:12" ht="52.5" customHeight="1">
-      <c r="G3" s="231"/>
-      <c r="H3" s="231"/>
-      <c r="I3" s="231"/>
-      <c r="J3" s="231"/>
-      <c r="K3" s="231"/>
-      <c r="L3" s="231"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="232"/>
+      <c r="I3" s="232"/>
+      <c r="J3" s="232"/>
+      <c r="K3" s="232"/>
+      <c r="L3" s="232"/>
     </row>
     <row r="5" spans="6:12" ht="18">
-      <c r="F5" s="233" t="s">
+      <c r="F5" s="234" t="s">
         <v>197</v>
       </c>
-      <c r="G5" s="234"/>
-      <c r="H5" s="234"/>
-      <c r="I5" s="234"/>
+      <c r="G5" s="235"/>
+      <c r="H5" s="235"/>
+      <c r="I5" s="235"/>
     </row>
     <row r="6" spans="6:12" ht="63">
       <c r="F6" s="48" t="s">
@@ -8452,13 +8476,13 @@
       <c r="F7" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="235" t="s">
+      <c r="G7" s="236" t="s">
         <v>142</v>
       </c>
       <c r="H7" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="I7" s="236" t="s">
+      <c r="I7" s="237" t="s">
         <v>202</v>
       </c>
       <c r="J7" s="54">
@@ -8469,11 +8493,11 @@
       <c r="F8" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="G8" s="235"/>
+      <c r="G8" s="236"/>
       <c r="H8" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="I8" s="236"/>
+      <c r="I8" s="237"/>
       <c r="J8" s="54">
         <v>1993.95</v>
       </c>
@@ -8576,7 +8600,7 @@
       <c r="H15" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="I15" s="237" t="s">
+      <c r="I15" s="238" t="s">
         <v>296</v>
       </c>
       <c r="J15" s="68">
@@ -8591,7 +8615,7 @@
       <c r="H16" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="I16" s="238"/>
+      <c r="I16" s="239"/>
       <c r="J16" s="68">
         <v>3849.3</v>
       </c>
@@ -8600,11 +8624,11 @@
       <c r="F17" s="69" t="s">
         <v>217</v>
       </c>
-      <c r="G17" s="239"/>
+      <c r="G17" s="240"/>
       <c r="H17" s="70" t="s">
         <v>218</v>
       </c>
-      <c r="I17" s="232" t="s">
+      <c r="I17" s="233" t="s">
         <v>219</v>
       </c>
       <c r="J17" s="71">
@@ -8615,11 +8639,11 @@
       <c r="F18" s="69" t="s">
         <v>220</v>
       </c>
-      <c r="G18" s="239"/>
+      <c r="G18" s="240"/>
       <c r="H18" s="70" t="s">
         <v>221</v>
       </c>
-      <c r="I18" s="232"/>
+      <c r="I18" s="233"/>
       <c r="J18" s="71">
         <v>4141.2</v>
       </c>
@@ -8705,11 +8729,11 @@
       </c>
     </row>
     <row r="4" spans="4:6" ht="26.25">
-      <c r="D4" s="241" t="s">
+      <c r="D4" s="242" t="s">
         <v>333</v>
       </c>
-      <c r="E4" s="241"/>
-      <c r="F4" s="241"/>
+      <c r="E4" s="242"/>
+      <c r="F4" s="242"/>
     </row>
     <row r="5" spans="4:6" ht="23.25">
       <c r="D5" s="16" t="s">
@@ -8794,11 +8818,11 @@
       <c r="F12" s="17"/>
     </row>
     <row r="18" spans="4:6" ht="31.5">
-      <c r="D18" s="240" t="s">
+      <c r="D18" s="241" t="s">
         <v>332</v>
       </c>
-      <c r="E18" s="240"/>
-      <c r="F18" s="240"/>
+      <c r="E18" s="241"/>
+      <c r="F18" s="241"/>
     </row>
     <row r="19" spans="4:6" ht="23.25">
       <c r="D19" s="16" t="s">
@@ -8858,7 +8882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -8875,7 +8899,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75">
-      <c r="B3" s="242" t="s">
+      <c r="B3" s="169" t="s">
         <v>436</v>
       </c>
     </row>
@@ -8885,7 +8909,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
-      <c r="B6" s="242" t="s">
+      <c r="B6" s="169" t="s">
         <v>437</v>
       </c>
     </row>

</xml_diff>